<commit_message>
final updates to new set up of unit models. reads in params from .csv straight to unit model. see storage and sulfur addition for examples. Carlsbad train partly complete -- all unit models need to be updated for trains to work and run. Results need to be double checked for errors
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksitterl/Documents/Python/watertap3/WaterTap3_repo/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5AC5A09-1BC5-C042-B48F-BA7254DBAB8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63FC147-B45D-8D45-A0CD-C43726EA0499}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="38680" windowHeight="21140" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="8780" yWindow="1520" windowWidth="38680" windowHeight="21140" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="91">
   <si>
     <t>outlet</t>
   </si>
@@ -292,13 +292,28 @@
   </si>
   <si>
     <t>{"hours": 6}</t>
+  </si>
+  <si>
+    <t>chemical_addition</t>
+  </si>
+  <si>
+    <t>{"chemical_name": "Sulphuric_Acid_H2SO4"}</t>
+  </si>
+  <si>
+    <t>breal</t>
+  </si>
+  <si>
+    <t>{"chemical_name": ["Sulphuric_Acid_H2SO4"]}</t>
+  </si>
+  <si>
+    <t>treated_storage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -335,6 +350,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -356,13 +377,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,12 +699,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A78" sqref="A78:XFD96"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -727,142 +749,138 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="G2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="D4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3"/>
+      <c r="D6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
@@ -872,24 +890,26 @@
         <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -899,26 +919,24 @@
         <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -928,26 +946,24 @@
         <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
@@ -957,24 +973,26 @@
         <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I10" s="3"/>
+      <c r="I10" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
@@ -984,19 +1002,19 @@
         <v>22</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>0</v>
@@ -1011,19 +1029,19 @@
         <v>22</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>0</v>
@@ -1038,24 +1056,26 @@
         <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I13" s="3"/>
+      <c r="I13" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -1065,25 +1085,25 @@
         <v>22</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1094,19 +1114,23 @@
         <v>22</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1117,22 +1141,22 @@
         <v>22</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="I16" s="3"/>
     </row>
@@ -1144,19 +1168,23 @@
         <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1167,19 +1195,23 @@
         <v>22</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1190,16 +1222,16 @@
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>12</v>
@@ -1208,7 +1240,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1219,26 +1251,20 @@
         <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
@@ -1248,26 +1274,24 @@
         <v>22</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
@@ -1277,16 +1301,16 @@
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1300,30 +1324,30 @@
         <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>44</v>
+      <c r="A24" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>1</v>
@@ -1335,124 +1359,118 @@
         <v>1</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I24" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3"/>
-    </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>44</v>
+      <c r="A26" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>9</v>
+        <v>34</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>9</v>
+        <v>27</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I26" s="3"/>
+      <c r="I26" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>44</v>
+      <c r="A27" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>67</v>
+        <v>33</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>44</v>
+      <c r="A28" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
@@ -1465,21 +1483,23 @@
         <v>21</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>15</v>
+        <v>27</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I29" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
@@ -1491,20 +1511,20 @@
       <c r="C30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>13</v>
+      <c r="D30" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>13</v>
+        <v>56</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="I30" s="3"/>
     </row>
@@ -1519,16 +1539,16 @@
         <v>21</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>5</v>
+        <v>75</v>
       </c>
       <c r="H31" s="3" t="s">
         <v>0</v>
@@ -1546,23 +1566,21 @@
         <v>21</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>6</v>
+        <v>75</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="H32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I32" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
@@ -1574,22 +1592,24 @@
       <c r="C33" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>6</v>
+      <c r="D33" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="H33" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I33" s="3"/>
+      <c r="I33" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
@@ -1601,20 +1621,20 @@
       <c r="C34" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>46</v>
+      <c r="D34" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="I34" s="3"/>
     </row>
@@ -1628,20 +1648,20 @@
       <c r="C35" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>57</v>
+      <c r="D35" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>57</v>
+        <v>13</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="I35" s="3"/>
     </row>
@@ -1656,16 +1676,16 @@
         <v>21</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>0</v>
@@ -1682,22 +1702,24 @@
       <c r="C37" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D37" s="3" t="s">
-        <v>7</v>
+      <c r="D37" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>76</v>
+      <c r="F37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I37" s="3"/>
+      <c r="I37" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
@@ -1710,16 +1732,16 @@
         <v>21</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>67</v>
+        <v>6</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>0</v>
@@ -1736,17 +1758,17 @@
       <c r="C39" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>11</v>
+      <c r="D39" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>12</v>
+        <v>57</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>0</v>
@@ -1763,17 +1785,21 @@
       <c r="C40" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>12</v>
+      <c r="D40" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I40" s="3"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
@@ -1786,17 +1812,21 @@
       <c r="C41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="3" t="s">
-        <v>24</v>
+      <c r="D41" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
@@ -1810,16 +1840,20 @@
         <v>21</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I42" s="3"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
@@ -1832,24 +1866,22 @@
       <c r="C43" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D43" s="3" t="s">
-        <v>1</v>
+      <c r="D43" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>66</v>
+        <v>11</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="I43" s="3"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="5" t="s">
@@ -1861,17 +1893,17 @@
       <c r="C44" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>56</v>
+      <c r="D44" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>60</v>
+        <v>11</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>0</v>
@@ -1888,21 +1920,17 @@
       <c r="C45" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>9</v>
+      <c r="D45" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
       <c r="I45" s="3"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -1915,21 +1943,17 @@
       <c r="C46" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>67</v>
+      <c r="D46" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="H46" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -1943,23 +1967,17 @@
         <v>21</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H47" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I47" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="5" t="s">
@@ -1972,21 +1990,23 @@
         <v>21</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>48</v>
+        <v>27</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I48" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
@@ -1998,20 +2018,20 @@
       <c r="C49" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>13</v>
+      <c r="D49" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="I49" s="3"/>
     </row>
@@ -2026,16 +2046,16 @@
         <v>21</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>0</v>
@@ -2053,23 +2073,21 @@
         <v>21</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>51</v>
+        <v>77</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I51" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="5" t="s">
@@ -2081,22 +2099,24 @@
       <c r="C52" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>6</v>
+      <c r="D52" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I52" s="3"/>
+      <c r="I52" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
@@ -2109,23 +2129,21 @@
         <v>21</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F53" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G53" s="5" t="s">
-        <v>62</v>
+        <v>28</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I53" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="5" t="s">
@@ -2137,20 +2155,20 @@
       <c r="C54" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>56</v>
+      <c r="D54" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G54" s="5" t="s">
-        <v>63</v>
+        <v>70</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="I54" s="3"/>
     </row>
@@ -2165,16 +2183,16 @@
         <v>21</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="E55" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G55" s="5" t="s">
-        <v>78</v>
+        <v>49</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>0</v>
@@ -2192,21 +2210,23 @@
         <v>21</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G56" s="5" t="s">
-        <v>72</v>
+        <v>50</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I56" s="3"/>
+      <c r="I56" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
@@ -2218,24 +2238,22 @@
       <c r="C57" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D57" s="3" t="s">
-        <v>46</v>
+      <c r="D57" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G57" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I57" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="I57" s="3"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="5" t="s">
@@ -2248,21 +2266,23 @@
         <v>21</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>64</v>
+        <v>27</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I58" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
@@ -2274,20 +2294,20 @@
       <c r="C59" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D59" s="3" t="s">
-        <v>13</v>
+      <c r="D59" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>74</v>
+        <v>62</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="I59" s="3"/>
     </row>
@@ -2302,16 +2322,16 @@
         <v>21</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>45</v>
+        <v>9</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="H60" s="3" t="s">
         <v>0</v>
@@ -2329,23 +2349,21 @@
         <v>21</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="H61" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I61" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I61" s="3"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="5" t="s">
@@ -2357,26 +2375,28 @@
       <c r="C62" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>6</v>
+      <c r="D62" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I62" s="3"/>
+      <c r="I62" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>22</v>
@@ -2385,27 +2405,25 @@
         <v>21</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>1</v>
+        <v>28</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>3</v>
+        <v>64</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I63" s="3"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>22</v>
@@ -2414,24 +2432,25 @@
         <v>21</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>3</v>
+      <c r="F64" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I64" s="3"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>22</v>
@@ -2439,25 +2458,26 @@
       <c r="C65" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D65" s="3" t="s">
-        <v>56</v>
+      <c r="D65" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>9</v>
+      <c r="F65" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="I65" s="3"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>22</v>
@@ -2465,25 +2485,28 @@
       <c r="C66" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D66" s="3" t="s">
-        <v>9</v>
+      <c r="D66" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>80</v>
+      <c r="F66" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>22</v>
@@ -2491,21 +2514,22 @@
       <c r="C67" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>80</v>
+      <c r="D67" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>80</v>
+      <c r="F67" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="I67" s="3"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
@@ -2518,19 +2542,22 @@
         <v>21</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -2544,19 +2571,19 @@
         <v>21</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -2570,16 +2597,16 @@
         <v>21</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H70" s="3" t="s">
         <v>0</v>
@@ -2596,16 +2623,16 @@
         <v>21</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>0</v>
@@ -2622,16 +2649,16 @@
         <v>21</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>0</v>
@@ -2648,16 +2675,16 @@
         <v>21</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>0</v>
@@ -2674,22 +2701,19 @@
         <v>21</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>12</v>
+        <v>82</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -2703,13 +2727,19 @@
         <v>21</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -2723,21 +2753,20 @@
         <v>21</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I76" s="3"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="5" t="s">
@@ -2750,146 +2779,141 @@
         <v>21</v>
       </c>
       <c r="D77" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A78" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A79" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A80" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A81" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I81" s="3"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A82" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D82" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E82" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="F82" s="3" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>83</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G78" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H78" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I78" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>83</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E79" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F79" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G79" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H79" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>83</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C80" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>83</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F81" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>83</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C82" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G82" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H82" s="3" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -2903,19 +2927,22 @@
         <v>21</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -2929,19 +2956,19 @@
         <v>21</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>84</v>
+        <v>56</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -2954,23 +2981,20 @@
       <c r="C85" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D85" s="5" t="s">
-        <v>5</v>
+      <c r="D85" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F85" s="5" t="s">
-        <v>5</v>
+      <c r="F85" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -2984,22 +3008,19 @@
         <v>21</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -3012,22 +3033,21 @@
       <c r="C87" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D87" s="5" t="s">
-        <v>17</v>
+      <c r="D87" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="E87" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="H87" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I87" s="3"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
@@ -3040,16 +3060,16 @@
         <v>21</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="H88" s="3" t="s">
         <v>0</v>
@@ -3066,19 +3086,19 @@
         <v>21</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
@@ -3091,20 +3111,23 @@
       <c r="C90" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D90" s="3" t="s">
-        <v>81</v>
+      <c r="D90" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F90" s="3" t="s">
-        <v>81</v>
+      <c r="F90" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3118,19 +3141,22 @@
         <v>21</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3143,24 +3169,22 @@
       <c r="C92" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>11</v>
+      <c r="D92" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I92" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="I92" s="3"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
@@ -3173,13 +3197,19 @@
         <v>21</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H93" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
@@ -3193,21 +3223,20 @@
         <v>21</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>13</v>
+        <v>60</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="H94" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I94" s="3"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
@@ -3220,13 +3249,19 @@
         <v>21</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>24</v>
+        <v>81</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>24</v>
+        <v>81</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H95" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
@@ -3240,19 +3275,142 @@
         <v>21</v>
       </c>
       <c r="D96" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H96" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>83</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H97" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>83</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>83</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H99" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I99" s="3"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>83</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>83</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E101" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F96" s="3" t="s">
+      <c r="F101" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
+      <c r="G101" s="3"/>
+      <c r="H101" s="3"/>
+      <c r="I101" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final checks complete for partial Carlsbad case. complete case to be finished tomorrow but format should be final
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63FC147-B45D-8D45-A0CD-C43726EA0499}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2E374D-0C35-D84A-A197-696997C59B3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8780" yWindow="1520" windowWidth="38680" windowHeight="21140" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="11200" yWindow="1540" windowWidth="38680" windowHeight="21140" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="91">
   <si>
     <t>outlet</t>
   </si>
@@ -699,12 +699,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>0</v>
@@ -789,23 +789,21 @@
         <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
@@ -818,23 +816,21 @@
         <v>21</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>28</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>90</v>
+        <v>6</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="6" t="s">
-        <v>31</v>
-      </c>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -847,17 +843,23 @@
         <v>21</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -870,212 +872,124 @@
         <v>21</v>
       </c>
       <c r="D6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="H6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
@@ -1088,22 +1002,22 @@
         <v>88</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1117,16 +1031,16 @@
         <v>88</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>0</v>
@@ -1144,19 +1058,19 @@
         <v>88</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="I16" s="3"/>
     </row>
@@ -1171,21 +1085,23 @@
         <v>88</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
@@ -1198,16 +1114,16 @@
         <v>88</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>0</v>
@@ -1225,23 +1141,21 @@
         <v>88</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="3" t="s">
-        <v>31</v>
-      </c>
+      <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
@@ -1254,17 +1168,23 @@
         <v>88</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+        <v>6</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
@@ -1277,21 +1197,23 @@
         <v>88</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I21" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
@@ -1304,16 +1226,20 @@
         <v>88</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1327,16 +1253,20 @@
         <v>88</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+        <v>8</v>
+      </c>
+      <c r="G23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1347,26 +1277,24 @@
         <v>22</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I24" s="3" t="s">
-        <v>35</v>
-      </c>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -1376,26 +1304,24 @@
         <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I25" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
@@ -1405,16 +1331,16 @@
         <v>22</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>34</v>
+        <v>88</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>12</v>
@@ -1423,7 +1349,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1434,7 +1360,7 @@
         <v>22</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>12</v>
@@ -1457,212 +1383,202 @@
         <v>22</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="H32" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F34" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H34" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>44</v>
+      <c r="A35" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
@@ -1675,22 +1591,24 @@
       <c r="C36" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>45</v>
+      <c r="D36" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>45</v>
+        <v>27</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="H36" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I36" s="3"/>
+      <c r="I36" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
@@ -1703,23 +1621,21 @@
         <v>21</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="H37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I37" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
@@ -1732,16 +1648,16 @@
         <v>21</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="H38" s="3" t="s">
         <v>0</v>
@@ -1759,16 +1675,16 @@
         <v>21</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>57</v>
+        <v>75</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="H39" s="3" t="s">
         <v>0</v>
@@ -1785,22 +1701,24 @@
       <c r="C40" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>57</v>
+      <c r="D40" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I40" s="3"/>
+      <c r="I40" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
@@ -1812,20 +1730,20 @@
       <c r="C41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>8</v>
+      <c r="D41" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="I41" s="3"/>
     </row>
@@ -1840,19 +1758,19 @@
         <v>21</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>76</v>
+      <c r="F42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="I42" s="3"/>
     </row>
@@ -1867,16 +1785,16 @@
         <v>21</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="H43" s="3" t="s">
         <v>0</v>
@@ -1893,22 +1811,24 @@
       <c r="C44" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D44" s="3" t="s">
-        <v>11</v>
+      <c r="D44" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I44" s="3"/>
+      <c r="I44" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="5" t="s">
@@ -1920,17 +1840,21 @@
       <c r="C45" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="3" t="s">
-        <v>12</v>
+      <c r="D45" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I45" s="3"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
@@ -1943,17 +1867,21 @@
       <c r="C46" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>24</v>
+      <c r="D46" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
@@ -1966,17 +1894,21 @@
       <c r="C47" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D47" s="3" t="s">
-        <v>14</v>
+      <c r="D47" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>0</v>
+      </c>
       <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
@@ -1989,24 +1921,22 @@
       <c r="C48" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="3" t="s">
-        <v>1</v>
+      <c r="D48" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="H48" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I48" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="I48" s="3"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="5" t="s">
@@ -2018,17 +1948,17 @@
       <c r="C49" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>56</v>
+      <c r="D49" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F49" s="5" t="s">
-        <v>59</v>
+      <c r="F49" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="H49" s="3" t="s">
         <v>0</v>
@@ -2046,16 +1976,16 @@
         <v>21</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>60</v>
+        <v>76</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="H50" s="3" t="s">
         <v>0</v>
@@ -2072,17 +2002,17 @@
       <c r="C51" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>67</v>
+      <c r="D51" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>68</v>
+        <v>11</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>0</v>
@@ -2100,23 +2030,17 @@
         <v>21</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I52" s="3" t="s">
-        <v>47</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="5" t="s">
@@ -2129,20 +2053,16 @@
         <v>21</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
       <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
@@ -2156,20 +2076,16 @@
         <v>21</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="G54" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
       <c r="I54" s="3"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
@@ -2182,22 +2098,24 @@
       <c r="C55" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>45</v>
+      <c r="D55" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>49</v>
+        <v>27</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I55" s="3"/>
+      <c r="I55" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="5" t="s">
@@ -2210,23 +2128,21 @@
         <v>21</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>60</v>
       </c>
       <c r="H56" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I56" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I56" s="3"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="5" t="s">
@@ -2239,16 +2155,16 @@
         <v>21</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="H57" s="3" t="s">
         <v>0</v>
@@ -2265,24 +2181,22 @@
       <c r="C58" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D58" s="3" t="s">
-        <v>1</v>
+      <c r="D58" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>71</v>
+        <v>28</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="H58" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I58" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="I58" s="3"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="5" t="s">
@@ -2294,22 +2208,24 @@
       <c r="C59" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>56</v>
+      <c r="D59" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G59" s="5" t="s">
-        <v>63</v>
+        <v>68</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="H59" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I59" s="3"/>
+      <c r="I59" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="5" t="s">
@@ -2321,20 +2237,20 @@
       <c r="C60" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>9</v>
+      <c r="D60" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>78</v>
+        <v>48</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="I60" s="3"/>
     </row>
@@ -2348,20 +2264,20 @@
       <c r="C61" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>67</v>
+      <c r="D61" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="I61" s="3"/>
     </row>
@@ -2375,24 +2291,22 @@
       <c r="C62" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>46</v>
+      <c r="D62" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="G62" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="H62" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I62" s="3" t="s">
-        <v>47</v>
-      </c>
+      <c r="I62" s="3"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="5" t="s">
@@ -2404,22 +2318,24 @@
       <c r="C63" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D63" s="3" t="s">
-        <v>15</v>
+      <c r="D63" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I63" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="5" t="s">
@@ -2431,20 +2347,20 @@
       <c r="C64" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D64" s="3" t="s">
-        <v>13</v>
+      <c r="D64" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="I64" s="3"/>
     </row>
@@ -2458,22 +2374,24 @@
       <c r="C65" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>45</v>
+      <c r="D65" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>53</v>
+        <v>27</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I65" s="3"/>
+      <c r="I65" s="3" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="5" t="s">
@@ -2486,23 +2404,21 @@
         <v>21</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I66" s="3" t="s">
-        <v>32</v>
-      </c>
+      <c r="I66" s="3"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="5" t="s">
@@ -2515,16 +2431,16 @@
         <v>21</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>0</v>
@@ -2533,7 +2449,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>22</v>
@@ -2541,28 +2457,26 @@
       <c r="C68" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>1</v>
+      <c r="D68" s="5" t="s">
+        <v>67</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>3</v>
+        <v>28</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="H68" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I68" s="3" t="s">
-        <v>36</v>
-      </c>
+      <c r="I68" s="3"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>22</v>
@@ -2571,24 +2485,27 @@
         <v>21</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F69" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>56</v>
+      <c r="F69" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="H69" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B70" s="3" t="s">
         <v>22</v>
@@ -2597,24 +2514,25 @@
         <v>21</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>56</v>
+        <v>15</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>56</v>
+      <c r="F70" s="5" t="s">
+        <v>52</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="H70" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I70" s="3"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B71" s="3" t="s">
         <v>22</v>
@@ -2623,24 +2541,25 @@
         <v>21</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>9</v>
+      <c r="F71" s="5" t="s">
+        <v>73</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="H71" s="3" t="s">
-        <v>0</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="I71" s="3"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B72" s="3" t="s">
         <v>22</v>
@@ -2648,25 +2567,26 @@
       <c r="C72" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>80</v>
+      <c r="D72" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>67</v>
+      <c r="F72" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="I72" s="3"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B73" s="3" t="s">
         <v>22</v>
@@ -2674,25 +2594,28 @@
       <c r="C73" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D73" s="3" t="s">
-        <v>67</v>
+      <c r="D73" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G73" s="3" t="s">
-        <v>15</v>
+      <c r="F73" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="H73" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="5" t="s">
-        <v>79</v>
+        <v>44</v>
       </c>
       <c r="B74" s="3" t="s">
         <v>22</v>
@@ -2700,21 +2623,22 @@
       <c r="C74" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D74" s="3" t="s">
-        <v>15</v>
+      <c r="D74" s="5" t="s">
+        <v>6</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>15</v>
+      <c r="F74" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I74" s="3"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="5" t="s">
@@ -2727,19 +2651,22 @@
         <v>21</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H75" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -2753,16 +2680,16 @@
         <v>21</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="H76" s="3" t="s">
         <v>0</v>
@@ -2779,16 +2706,16 @@
         <v>21</v>
       </c>
       <c r="D77" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F77" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="H77" s="3" t="s">
         <v>0</v>
@@ -2805,16 +2732,16 @@
         <v>21</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="E78" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="H78" s="3" t="s">
         <v>0</v>
@@ -2831,22 +2758,19 @@
         <v>21</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="H79" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="I79" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -2860,13 +2784,19 @@
         <v>21</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>12</v>
+        <v>67</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>12</v>
+        <v>67</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -2880,21 +2810,20 @@
         <v>21</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>15</v>
+        <v>82</v>
       </c>
       <c r="H81" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I81" s="3"/>
+        <v>41</v>
+      </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="5" t="s">
@@ -2907,18 +2836,24 @@
         <v>21</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A83" t="s">
-        <v>83</v>
+      <c r="A83" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="B83" s="3" t="s">
         <v>22</v>
@@ -2927,27 +2862,24 @@
         <v>21</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="H83" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I83" s="3" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>83</v>
+      <c r="A84" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="B84" s="3" t="s">
         <v>22</v>
@@ -2956,24 +2888,24 @@
         <v>21</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E84" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="H84" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
-        <v>83</v>
+      <c r="A85" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="B85" s="3" t="s">
         <v>22</v>
@@ -2982,24 +2914,24 @@
         <v>21</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="E85" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>56</v>
+        <v>81</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H85" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
-        <v>83</v>
+      <c r="A86" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>22</v>
@@ -3008,24 +2940,27 @@
         <v>21</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E86" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="H86" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="I86" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A87" t="s">
-        <v>83</v>
+      <c r="A87" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>22</v>
@@ -3034,24 +2969,18 @@
         <v>21</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>80</v>
+        <v>12</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G87" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H87" s="3" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A88" t="s">
-        <v>83</v>
+      <c r="A88" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="B88" s="3" t="s">
         <v>22</v>
@@ -3060,13 +2989,13 @@
         <v>21</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>67</v>
+        <v>13</v>
       </c>
       <c r="G88" s="3" t="s">
         <v>15</v>
@@ -3074,10 +3003,11 @@
       <c r="H88" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="I88" s="3"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
-        <v>83</v>
+      <c r="A89" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="B89" s="3" t="s">
         <v>22</v>
@@ -3086,19 +3016,13 @@
         <v>21</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
@@ -3111,23 +3035,23 @@
       <c r="C90" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D90" s="5" t="s">
-        <v>5</v>
+      <c r="D90" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>5</v>
+        <v>27</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>1</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3141,22 +3065,19 @@
         <v>21</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E91" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="I91" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
@@ -3169,22 +3090,21 @@
       <c r="C92" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D92" s="5" t="s">
-        <v>17</v>
+      <c r="D92" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="E92" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="H92" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I92" s="3"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
@@ -3197,16 +3117,16 @@
         <v>21</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H93" s="3" t="s">
         <v>0</v>
@@ -3223,16 +3143,16 @@
         <v>21</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="E94" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="H94" s="3" t="s">
         <v>0</v>
@@ -3249,16 +3169,16 @@
         <v>21</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="E95" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H95" s="3" t="s">
         <v>0</v>
@@ -3275,19 +3195,19 @@
         <v>21</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E96" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.2">
@@ -3300,23 +3220,23 @@
       <c r="C97" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D97" s="3" t="s">
-        <v>11</v>
+      <c r="D97" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="E97" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>11</v>
+      <c r="F97" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.2">
@@ -3330,13 +3250,22 @@
         <v>21</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>12</v>
+        <v>6</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.2">
@@ -3349,20 +3278,20 @@
       <c r="C99" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D99" s="3" t="s">
-        <v>13</v>
+      <c r="D99" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="E99" s="3" t="s">
         <v>28</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="H99" s="3" t="s">
-        <v>41</v>
+        <v>0</v>
       </c>
       <c r="I99" s="3"/>
     </row>
@@ -3377,13 +3306,19 @@
         <v>21</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>24</v>
+        <v>7</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.2">
@@ -3397,17 +3332,191 @@
         <v>21</v>
       </c>
       <c r="D101" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>83</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>83</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H103" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>83</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>83</v>
+      </c>
+      <c r="B105" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>83</v>
+      </c>
+      <c r="B106" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H106" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I106" s="3"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>83</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>83</v>
+      </c>
+      <c r="B108" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D108" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E108" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F101" s="3" t="s">
+      <c r="F108" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
+      <c r="G108" s="3"/>
+      <c r="H108" s="3"/>
+      <c r="I108" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>

</xml_diff>

<commit_message>
fixing Carlsbad data inputs, and units in coag_floc and sodium_bi
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CECCFA2-42EC-B843-A5D1-31EC6DBF9989}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F38899A-15E5-5E46-B727-EC2893BC57B6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15640" yWindow="1560" windowWidth="33660" windowHeight="23000" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="6020" yWindow="760" windowWidth="33660" windowHeight="23000" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="94">
   <si>
     <t>outlet</t>
   </si>
@@ -313,6 +313,9 @@
   </si>
   <si>
     <t>chlorination</t>
+  </si>
+  <si>
+    <t>{"recovery": 0.95}</t>
   </si>
 </sst>
 </file>
@@ -715,10 +718,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19:XFD39"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1155,7 +1158,9 @@
       <c r="H15" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>

</xml_diff>

<commit_message>
changes to csvs and input file to make BW runs
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showObjects="none" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksitterl/Documents/Python/watertap3/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3DB9E86-66FC-E148-ADF9-C1DCB9A77C42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C4716F-9AF3-8B40-8CF1-37FFD580E607}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14080" yWindow="1240" windowWidth="36300" windowHeight="23980" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="40720" yWindow="1600" windowWidth="36900" windowHeight="18940" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="120">
   <si>
     <t>outlet</t>
   </si>
@@ -363,9 +363,6 @@
     <t>electrodialysis_reversal</t>
   </si>
   <si>
-    <t>treated_storage_b,irwin_brine_management</t>
-  </si>
-  <si>
     <t>treated_storage_b</t>
   </si>
   <si>
@@ -375,17 +372,35 @@
     <t>deep_well_injection</t>
   </si>
   <si>
-    <t>treated_storage_b,deep_well_injection</t>
-  </si>
-  <si>
     <t>{"incl_piping": ["True"]}</t>
+  </si>
+  <si>
+    <t>KBHDP</t>
+  </si>
+  <si>
+    <t>{"source_type": ["KBHDP_Brackish_Ave"]}</t>
+  </si>
+  <si>
+    <t>caustic_soda_addition,deep_well_injection</t>
+  </si>
+  <si>
+    <t>water_pumping_station</t>
+  </si>
+  <si>
+    <t>treated_storage,irwin_brine_management</t>
+  </si>
+  <si>
+    <t>municipal_drinking,water_pumping_station</t>
+  </si>
+  <si>
+    <t>{"pump_type": ["raw"], 'tdh': [125]}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -435,11 +450,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Apple Color Emoji"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -470,7 +480,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,12 +795,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
-  <dimension ref="A1:N119"/>
+  <dimension ref="A1:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="I119" sqref="I119"/>
+      <selection pane="bottomLeft" activeCell="I116" sqref="I116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4379,7 +4389,7 @@
         <v>108</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="H113" s="6" t="s">
         <v>39</v>
@@ -4402,22 +4412,22 @@
         <v>19</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="E114" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>10</v>
+        <v>109</v>
       </c>
       <c r="H114" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I114" s="6" t="s">
-        <v>77</v>
+      <c r="I114" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="J114" s="6"/>
       <c r="K114" s="6"/>
@@ -4436,21 +4446,23 @@
         <v>19</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="E115" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>6</v>
+        <v>109</v>
+      </c>
+      <c r="G115" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="H115" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I115" s="6"/>
+      <c r="I115" s="6" t="s">
+        <v>77</v>
+      </c>
       <c r="J115" s="6"/>
       <c r="K115" s="6"/>
       <c r="L115" s="6"/>
@@ -4467,22 +4479,24 @@
       <c r="C116" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D116" s="6" t="s">
-        <v>6</v>
+      <c r="D116" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="E116" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F116" s="6" t="s">
-        <v>6</v>
+      <c r="F116" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H116" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I116" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="I116" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="J116" s="6"/>
       <c r="K116" s="6"/>
       <c r="L116" s="6"/>
@@ -4500,16 +4514,20 @@
         <v>19</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="E117" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G117" s="6"/>
-      <c r="H117" s="6"/>
+        <v>105</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H117" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="I117" s="6"/>
       <c r="J117" s="6"/>
       <c r="K117" s="6"/>
@@ -4517,7 +4535,7 @@
       <c r="M117" s="6"/>
       <c r="N117" s="6"/>
     </row>
-    <row r="118" spans="1:14" ht="28" x14ac:dyDescent="0.5">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="6" t="s">
         <v>103</v>
       </c>
@@ -4528,17 +4546,26 @@
         <v>19</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>112</v>
+        <v>6</v>
       </c>
       <c r="E118" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F118" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="I118" s="8" t="s">
-        <v>114</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="H118" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I118" s="6"/>
+      <c r="J118" s="6"/>
+      <c r="K118" s="6"/>
+      <c r="L118" s="6"/>
+      <c r="M118" s="6"/>
+      <c r="N118" s="6"/>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="6" t="s">
@@ -4551,12 +4578,389 @@
         <v>19</v>
       </c>
       <c r="D119" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H119" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I119" s="6"/>
+      <c r="J119" s="6"/>
+      <c r="K119" s="6"/>
+      <c r="L119" s="6"/>
+      <c r="M119" s="6"/>
+      <c r="N119" s="6"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A120" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E120" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F120" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G120" s="6"/>
+      <c r="H120" s="6"/>
+      <c r="I120" s="6"/>
+      <c r="J120" s="6"/>
+      <c r="K120" s="6"/>
+      <c r="L120" s="6"/>
+      <c r="M120" s="6"/>
+      <c r="N120" s="6"/>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A121" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B121" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C121" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E121" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F121" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I121" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A122" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B122" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C122" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D122" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E119" s="6" t="s">
+      <c r="E122" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F119" s="6" t="s">
+      <c r="F122" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>113</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G123" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="H123" t="s">
+        <v>0</v>
+      </c>
+      <c r="I123" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>113</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C124" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E124" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F124" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G124" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H124" t="s">
+        <v>0</v>
+      </c>
+      <c r="I124"/>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
+        <v>113</v>
+      </c>
+      <c r="B125" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C125" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E125" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G125" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H125" t="s">
+        <v>0</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A126" t="s">
+        <v>113</v>
+      </c>
+      <c r="B126" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C126" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D126" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E126" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F126" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G126" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H126" t="s">
+        <v>0</v>
+      </c>
+      <c r="I126"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A127" t="s">
+        <v>113</v>
+      </c>
+      <c r="B127" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C127" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E127" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F127" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G127" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H127" t="s">
+        <v>39</v>
+      </c>
+      <c r="I127"/>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A128" t="s">
+        <v>113</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C128" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E128" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F128" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G128" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H128" t="s">
+        <v>0</v>
+      </c>
+      <c r="I128" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>113</v>
+      </c>
+      <c r="B129" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C129" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D129" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E129" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F129" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="G129" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H129" t="s">
+        <v>0</v>
+      </c>
+      <c r="I129" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>113</v>
+      </c>
+      <c r="B130" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C130" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="E130" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F130" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="G130" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H130" t="s">
+        <v>0</v>
+      </c>
+      <c r="I130" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
+        <v>113</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C131" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E131" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F131" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G131" s="6"/>
+      <c r="H131"/>
+      <c r="I131"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A132" t="s">
+        <v>113</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C132" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E132" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="G132"/>
+      <c r="H132"/>
+      <c r="I132" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A133" t="s">
+        <v>113</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C133" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E133" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F133" s="6" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change to input file to make Irwin run
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksitterl/Documents/Python/watertap3/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C4716F-9AF3-8B40-8CF1-37FFD580E607}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA72D459-69C7-2D4B-9F04-055943A4E019}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40720" yWindow="1600" windowWidth="36900" windowHeight="18940" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="39600" yWindow="1600" windowWidth="36900" windowHeight="18940" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="121">
   <si>
     <t>outlet</t>
   </si>
@@ -394,6 +394,9 @@
   </si>
   <si>
     <t>{"pump_type": ["raw"], 'tdh': [125]}</t>
+  </si>
+  <si>
+    <t>media_filtration_2</t>
   </si>
 </sst>
 </file>
@@ -797,10 +800,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:N133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="I116" sqref="I116"/>
+      <selection pane="bottomLeft" activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4489,7 +4492,7 @@
         <v>7</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="H116" s="6" t="s">
         <v>0</v>
@@ -4520,7 +4523,7 @@
         <v>26</v>
       </c>
       <c r="F117" s="6" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="G117" s="6" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
change to input file to make KBHDPDP run
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksitterl/Documents/Python/watertap3/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA72D459-69C7-2D4B-9F04-055943A4E019}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAD2260-C047-6C48-B434-0A033C2579F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39600" yWindow="1600" windowWidth="36900" windowHeight="18940" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1102" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="123">
   <si>
     <t>outlet</t>
   </si>
@@ -397,6 +397,12 @@
   </si>
   <si>
     <t>media_filtration_2</t>
+  </si>
+  <si>
+    <t>{"hours": 12}</t>
+  </si>
+  <si>
+    <t>{"incl_piping": ["True"], "pipe_distance": [22]}</t>
   </si>
 </sst>
 </file>
@@ -798,12 +804,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
-  <dimension ref="A1:N133"/>
+  <dimension ref="A1:N132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="H118" sqref="H118"/>
+      <selection pane="bottomLeft" activeCell="A127" sqref="A127:XFD127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4778,12 +4784,12 @@
         <v>6</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H126" t="s">
-        <v>0</v>
-      </c>
-      <c r="I126"/>
+        <v>115</v>
+      </c>
+      <c r="H126" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I126" s="6"/>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
@@ -4796,21 +4802,23 @@
         <v>19</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E127" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F127" s="6" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="G127" s="6" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="H127" t="s">
-        <v>39</v>
-      </c>
-      <c r="I127"/>
+        <v>0</v>
+      </c>
+      <c r="I127" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
@@ -4823,22 +4831,22 @@
         <v>19</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E128" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F128" s="6" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="G128" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H128" t="s">
         <v>0</v>
       </c>
       <c r="I128" s="6" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.2">
@@ -4852,22 +4860,22 @@
         <v>19</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E129" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F129" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="H129" t="s">
         <v>0</v>
       </c>
       <c r="I129" s="6" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.2">
@@ -4881,23 +4889,17 @@
         <v>19</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>79</v>
+        <v>10</v>
       </c>
       <c r="E130" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F130" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G130" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H130" t="s">
-        <v>0</v>
-      </c>
-      <c r="I130" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="G130" s="6"/>
+      <c r="H130"/>
+      <c r="I130"/>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
@@ -4910,17 +4912,19 @@
         <v>19</v>
       </c>
       <c r="D131" s="6" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
       <c r="E131" s="6" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F131" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G131" s="6"/>
+        <v>111</v>
+      </c>
+      <c r="G131"/>
       <c r="H131"/>
-      <c r="I131"/>
+      <c r="I131" s="5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
@@ -4933,37 +4937,12 @@
         <v>19</v>
       </c>
       <c r="D132" s="6" t="s">
-        <v>111</v>
+        <v>22</v>
       </c>
       <c r="E132" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F132" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G132"/>
-      <c r="H132"/>
-      <c r="I132" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>113</v>
-      </c>
-      <c r="B133" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C133" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D133" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E133" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F133" s="6" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to input file for Santa Barbara  and lime_softening.py
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksitterl/Documents/Python/watertap3/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAD2260-C047-6C48-B434-0A033C2579F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3760BF2B-C9DB-8A4B-B1BB-40DE55C9AAD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39600" yWindow="1600" windowWidth="36900" windowHeight="18940" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1094" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="120">
   <si>
     <t>outlet</t>
   </si>
@@ -129,15 +129,6 @@
     <t>{"membrane": "X"}</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>{"source_type": ["Seawater", "Brackish"]}</t>
-  </si>
-  <si>
     <t>{"source_type": ["Seawater"]}</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>anti_scalant_addition_3,backwash_solids_handling_3</t>
   </si>
   <si>
-    <t>holding_tank_a</t>
-  </si>
-  <si>
     <t>holding_tank_b</t>
   </si>
   <si>
@@ -237,12 +225,6 @@
     <t>tri_media_filtration_3,landfill</t>
   </si>
   <si>
-    <t>static_mix_a</t>
-  </si>
-  <si>
-    <t>static_mix_b</t>
-  </si>
-  <si>
     <t>static_mix_a_2</t>
   </si>
   <si>
@@ -279,9 +261,6 @@
     <t>{"chemical_name": ["Sodium_Bisullfite_NaHSO3"]}</t>
   </si>
   <si>
-    <t>{"chemical_name": ["Lime_Suspension_CaOH_2"]}</t>
-  </si>
-  <si>
     <t>{"chemical_name": ["Ammonia"]}</t>
   </si>
   <si>
@@ -312,9 +291,6 @@
     <t>{"chemical_name": ["Hydrazine_(N2H4)"]}</t>
   </si>
   <si>
-    <t>{"chemical_name": ["Hydrogen_Peroxide"], "uv_dose": [325], 'aop': ['True'], 'dose':[5]}</t>
-  </si>
-  <si>
     <t>fecl3_addition_a</t>
   </si>
   <si>
@@ -403,6 +379,21 @@
   </si>
   <si>
     <t>{"incl_piping": ["True"], "pipe_distance": [22]}</t>
+  </si>
+  <si>
+    <t>{"chemical_name": ["Lime_Suspension_CaOH_2"], "lime": [2.3]}</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>{"chemical_name": ["Hydrogen_Peroxide"], "uv_dose": [80], 'aop': ['True'], 'dose':[5]}</t>
+  </si>
+  <si>
+    <t>outlet,outlet,outlet</t>
+  </si>
+  <si>
+    <t>ro_deep,ro_deep_2,ro_deep_3</t>
   </si>
 </sst>
 </file>
@@ -804,17 +795,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
-  <dimension ref="A1:N132"/>
+  <dimension ref="A1:N126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="159" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A127" sqref="A127:XFD127"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="4"/>
     <col min="3" max="3" width="16.5" style="4" customWidth="1"/>
     <col min="4" max="4" width="30.83203125" style="4" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" style="4" customWidth="1"/>
@@ -842,13 +834,13 @@
         <v>24</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>28</v>
@@ -880,7 +872,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -930,10 +922,10 @@
         <v>13</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I4" s="5"/>
     </row>
@@ -963,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -992,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1104,7 +1096,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1127,7 +1119,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>0</v>
@@ -1145,22 +1137,22 @@
         <v>19</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1174,22 +1166,22 @@
         <v>19</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>79</v>
-      </c>
       <c r="H13" s="5" t="s">
         <v>0</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>82</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1203,13 +1195,13 @@
         <v>19</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>10</v>
@@ -1218,7 +1210,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -1241,13 +1233,13 @@
         <v>11</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
@@ -1324,141 +1316,175 @@
       <c r="K18" s="6"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="A19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I19" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A20" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="A21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="A22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="A23" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>20</v>
@@ -1467,23 +1493,21 @@
         <v>19</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>87</v>
+        <v>13</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I24" s="6"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -1492,7 +1516,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>20</v>
@@ -1500,23 +1524,23 @@
       <c r="C25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>87</v>
+      <c r="D25" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F25" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>84</v>
+      <c r="F25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="H25" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I25" s="6" t="s">
-        <v>88</v>
+      <c r="I25" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
@@ -1526,7 +1550,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>20</v>
@@ -1535,22 +1559,22 @@
         <v>19</v>
       </c>
       <c r="D26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
@@ -1560,7 +1584,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>20</v>
@@ -1569,21 +1593,23 @@
         <v>19</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>58</v>
+        <v>5</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I27" s="6"/>
+        <v>118</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
@@ -1592,7 +1618,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>20</v>
@@ -1600,24 +1626,22 @@
       <c r="C28" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D28" s="6" t="s">
-        <v>43</v>
+      <c r="D28" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>13</v>
+        <v>6</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I28" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="I28" s="6"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
@@ -1626,7 +1650,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>20</v>
@@ -1634,20 +1658,20 @@
       <c r="C29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>13</v>
+      <c r="D29" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
@@ -1658,7 +1682,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>20</v>
@@ -1666,24 +1690,22 @@
       <c r="C30" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>11</v>
+      <c r="D30" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>40</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>85</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
@@ -1692,7 +1714,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>20</v>
@@ -1701,22 +1723,22 @@
         <v>19</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
@@ -1726,7 +1748,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>20</v>
@@ -1735,22 +1757,22 @@
         <v>19</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H32" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>30</v>
+        <v>117</v>
       </c>
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
@@ -1760,7 +1782,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>20</v>
@@ -1769,16 +1791,16 @@
         <v>19</v>
       </c>
       <c r="D33" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>0</v>
@@ -1792,7 +1814,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>20</v>
@@ -1800,23 +1822,23 @@
       <c r="C34" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="7" t="s">
-        <v>43</v>
+      <c r="D34" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>59</v>
+      <c r="F34" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I34" s="6" t="s">
-        <v>90</v>
+      <c r="I34" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -1826,7 +1848,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>20</v>
@@ -1834,23 +1856,23 @@
       <c r="C35" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>53</v>
+      <c r="D35" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F35" s="7" t="s">
-        <v>53</v>
+      <c r="F35" s="6" t="s">
+        <v>101</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="J35" s="6"/>
       <c r="K35" s="6"/>
@@ -1860,7 +1882,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>20</v>
@@ -1868,21 +1890,17 @@
       <c r="C36" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>8</v>
+      <c r="D36" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
       <c r="K36" s="6"/>
@@ -1892,7 +1910,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>20</v>
@@ -1901,23 +1919,17 @@
         <v>19</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I37" s="6" t="s">
-        <v>81</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6"/>
       <c r="L37" s="6"/>
@@ -1926,7 +1938,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>20</v>
@@ -1934,22 +1946,24 @@
       <c r="C38" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="7" t="s">
-        <v>89</v>
+      <c r="D38" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>68</v>
+        <v>25</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I38" s="6"/>
+      <c r="I38" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6"/>
       <c r="L38" s="6"/>
@@ -1958,31 +1972,31 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E39" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>10</v>
-      </c>
       <c r="H39" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
@@ -1992,26 +2006,32 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
+      <c r="G40" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="J40" s="6"/>
       <c r="K40" s="6"/>
       <c r="L40" s="6"/>
@@ -2020,7 +2040,7 @@
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>20</v>
@@ -2028,17 +2048,21 @@
       <c r="C41" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="6" t="s">
-        <v>22</v>
+      <c r="D41" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
@@ -2048,7 +2072,7 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>20</v>
@@ -2057,17 +2081,23 @@
         <v>19</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
@@ -2076,7 +2106,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>20</v>
@@ -2085,23 +2115,21 @@
         <v>19</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>35</v>
+        <v>26</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
       <c r="L43" s="6"/>
@@ -2110,7 +2138,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>20</v>
@@ -2118,23 +2146,23 @@
       <c r="C44" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="7" t="s">
-        <v>87</v>
+      <c r="D44" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>94</v>
+        <v>58</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>88</v>
+        <v>36</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="J44" s="6"/>
       <c r="K44" s="6"/>
@@ -2144,7 +2172,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>20</v>
@@ -2153,22 +2181,22 @@
         <v>19</v>
       </c>
       <c r="D45" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I45" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="G45" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="J45" s="6"/>
       <c r="K45" s="6"/>
@@ -2178,7 +2206,7 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>20</v>
@@ -2187,21 +2215,23 @@
         <v>19</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>60</v>
+        <v>44</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="H46" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I46" s="6"/>
+      <c r="I46" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6"/>
       <c r="L46" s="6"/>
@@ -2210,7 +2240,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>20</v>
@@ -2218,24 +2248,22 @@
       <c r="C47" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>43</v>
+      <c r="D47" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I47" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="I47" s="6"/>
       <c r="J47" s="6"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
@@ -2244,7 +2272,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>20</v>
@@ -2253,21 +2281,23 @@
         <v>19</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="G48" s="6" t="s">
-        <v>55</v>
+        <v>25</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I48" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="J48" s="6"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
@@ -2276,7 +2306,7 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>20</v>
@@ -2284,23 +2314,23 @@
       <c r="C49" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="6" t="s">
-        <v>11</v>
+      <c r="D49" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="G49" s="6" t="s">
-        <v>61</v>
+        <v>53</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>85</v>
+        <v>0</v>
+      </c>
+      <c r="I49" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -2310,7 +2340,7 @@
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>20</v>
@@ -2319,22 +2349,22 @@
         <v>19</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>47</v>
+        <v>87</v>
+      </c>
+      <c r="G50" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="H50" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="J50" s="6"/>
       <c r="K50" s="6"/>
@@ -2344,7 +2374,7 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>20</v>
@@ -2353,23 +2383,21 @@
         <v>19</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>5</v>
+        <v>82</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="G51" s="6" t="s">
-        <v>48</v>
+        <v>64</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I51" s="6" t="s">
-        <v>30</v>
-      </c>
+      <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
@@ -2378,7 +2406,7 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>20</v>
@@ -2386,22 +2414,24 @@
       <c r="C52" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="7" t="s">
-        <v>6</v>
+      <c r="D52" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="G52" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="H52" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I52" s="6"/>
+      <c r="I52" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="J52" s="6"/>
       <c r="K52" s="6"/>
       <c r="L52" s="6"/>
@@ -2410,7 +2440,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>20</v>
@@ -2419,23 +2449,21 @@
         <v>19</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="G53" s="7" t="s">
-        <v>56</v>
+        <v>26</v>
+      </c>
+      <c r="F53" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>54</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I53" s="6"/>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
@@ -2444,7 +2472,7 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>20</v>
@@ -2452,23 +2480,23 @@
       <c r="C54" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D54" s="7" t="s">
-        <v>87</v>
+      <c r="D54" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="G54" s="7" t="s">
-        <v>95</v>
+        <v>61</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I54" s="6" t="s">
-        <v>88</v>
+        <v>36</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="J54" s="6"/>
       <c r="K54" s="6"/>
@@ -2478,7 +2506,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>20</v>
@@ -2487,22 +2515,22 @@
         <v>19</v>
       </c>
       <c r="D55" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I55" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="G55" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I55" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
@@ -2512,7 +2540,7 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>20</v>
@@ -2521,21 +2549,23 @@
         <v>19</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="G56" s="7" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I56" s="6"/>
+      <c r="I56" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J56" s="6"/>
       <c r="K56" s="6"/>
       <c r="L56" s="6"/>
@@ -2544,7 +2574,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>20</v>
@@ -2552,24 +2582,22 @@
       <c r="C57" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D57" s="6" t="s">
-        <v>43</v>
+      <c r="D57" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G57" s="7" t="s">
         <v>49</v>
       </c>
+      <c r="G57" s="6" t="s">
+        <v>55</v>
+      </c>
       <c r="H57" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I57" s="6" t="s">
-        <v>90</v>
-      </c>
+      <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
@@ -2578,7 +2606,7 @@
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>20</v>
@@ -2587,21 +2615,23 @@
         <v>19</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>49</v>
+        <v>25</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>1</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>57</v>
+        <v>3</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I58" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>31</v>
+      </c>
       <c r="J58" s="6"/>
       <c r="K58" s="6"/>
       <c r="L58" s="6"/>
@@ -2610,7 +2640,7 @@
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>20</v>
@@ -2619,22 +2649,22 @@
         <v>19</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E59" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F59" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="G59" s="6" t="s">
-        <v>66</v>
+      <c r="F59" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>85</v>
+        <v>0</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
@@ -2644,7 +2674,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>20</v>
@@ -2653,22 +2683,22 @@
         <v>19</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="E60" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G60" s="7" t="s">
-        <v>51</v>
+        <v>80</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I60" s="6" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="J60" s="6"/>
       <c r="K60" s="6"/>
@@ -2678,7 +2708,7 @@
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>20</v>
@@ -2686,23 +2716,23 @@
       <c r="C61" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="7" t="s">
-        <v>5</v>
+      <c r="D61" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="E61" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F61" s="7" t="s">
-        <v>51</v>
+      <c r="F61" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I61" s="6" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="J61" s="6"/>
       <c r="K61" s="6"/>
@@ -2712,7 +2742,7 @@
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>20</v>
@@ -2721,21 +2751,20 @@
         <v>19</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>6</v>
+        <v>82</v>
       </c>
       <c r="E62" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>59</v>
+        <v>13</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I62" s="6"/>
       <c r="J62" s="6"/>
       <c r="K62" s="6"/>
       <c r="L62" s="6"/>
@@ -2744,7 +2773,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>20</v>
@@ -2753,23 +2782,21 @@
         <v>19</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F63" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>3</v>
+        <v>68</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I63" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I63" s="6"/>
       <c r="J63" s="6"/>
       <c r="K63" s="6"/>
       <c r="L63" s="6"/>
@@ -2778,7 +2805,7 @@
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>20</v>
@@ -2787,23 +2814,21 @@
         <v>19</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G64" s="7" t="s">
-        <v>87</v>
+        <v>6</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I64" s="6" t="s">
-        <v>78</v>
-      </c>
+      <c r="I64" s="6"/>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
       <c r="L64" s="6"/>
@@ -2812,7 +2837,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>20</v>
@@ -2820,23 +2845,23 @@
       <c r="C65" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D65" s="7" t="s">
-        <v>87</v>
+      <c r="D65" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F65" s="7" t="s">
-        <v>87</v>
+      <c r="F65" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H65" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I65" s="6" t="s">
-        <v>83</v>
+      <c r="I65" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
@@ -2846,7 +2871,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>20</v>
@@ -2855,22 +2880,22 @@
         <v>19</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E66" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F66" s="6" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H66" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I66" s="6" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="J66" s="6"/>
       <c r="K66" s="6"/>
@@ -2880,7 +2905,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>20</v>
@@ -2889,22 +2914,22 @@
         <v>19</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="E67" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="H67" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I67" s="6" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
@@ -2914,7 +2939,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>20</v>
@@ -2922,23 +2947,23 @@
       <c r="C68" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D68" s="7" t="s">
-        <v>89</v>
+      <c r="D68" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="E68" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F68" s="7" t="s">
-        <v>89</v>
+      <c r="F68" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H68" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I68" s="6" t="s">
-        <v>88</v>
+        <v>41</v>
       </c>
       <c r="J68" s="6"/>
       <c r="K68" s="6"/>
@@ -2948,7 +2973,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>20</v>
@@ -2957,20 +2982,16 @@
         <v>19</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>39</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
@@ -2980,7 +3001,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>20</v>
@@ -2989,21 +3010,23 @@
         <v>19</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E70" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H70" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I70" s="6"/>
+      <c r="I70" s="5" t="s">
+        <v>78</v>
+      </c>
       <c r="J70" s="6"/>
       <c r="K70" s="6"/>
       <c r="L70" s="6"/>
@@ -3012,7 +3035,7 @@
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>20</v>
@@ -3021,23 +3044,17 @@
         <v>19</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F71" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G71" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H71" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I71" s="6" t="s">
-        <v>81</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
       <c r="J71" s="6"/>
       <c r="K71" s="6"/>
       <c r="L71" s="6"/>
@@ -3045,8 +3062,8 @@
       <c r="N71" s="6"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A72" s="7" t="s">
-        <v>71</v>
+      <c r="A72" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>20</v>
@@ -3055,22 +3072,22 @@
         <v>19</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>84</v>
+        <v>1</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F72" s="6" t="s">
-        <v>94</v>
+        <v>1</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="H72" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>83</v>
+        <v>31</v>
       </c>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
@@ -3079,8 +3096,8 @@
       <c r="N72" s="6"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="7" t="s">
-        <v>71</v>
+      <c r="A73" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>20</v>
@@ -3089,22 +3106,22 @@
         <v>19</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>73</v>
+        <v>3</v>
       </c>
       <c r="E73" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F73" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>79</v>
+        <v>3</v>
+      </c>
+      <c r="G73" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="H73" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
@@ -3113,8 +3130,8 @@
       <c r="N73" s="6"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A74" s="7" t="s">
-        <v>71</v>
+      <c r="A74" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>20</v>
@@ -3122,23 +3139,23 @@
       <c r="C74" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D74" s="6" t="s">
-        <v>79</v>
+      <c r="D74" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="E74" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F74" s="6" t="s">
-        <v>79</v>
+      <c r="F74" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="H74" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>44</v>
+        <v>81</v>
       </c>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
@@ -3147,8 +3164,8 @@
       <c r="N74" s="6"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A75" s="7" t="s">
-        <v>71</v>
+      <c r="A75" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>20</v>
@@ -3157,17 +3174,23 @@
         <v>19</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
+        <v>77</v>
+      </c>
+      <c r="G75" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I75" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
@@ -3175,8 +3198,8 @@
       <c r="N75" s="6"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A76" s="7" t="s">
-        <v>71</v>
+      <c r="A76" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B76" s="6" t="s">
         <v>20</v>
@@ -3185,22 +3208,22 @@
         <v>19</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="E76" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F76" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G76" s="6" t="s">
-        <v>13</v>
+        <v>66</v>
+      </c>
+      <c r="G76" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="H76" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I76" s="5" t="s">
-        <v>85</v>
+      <c r="I76" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="J76" s="6"/>
       <c r="K76" s="6"/>
@@ -3209,8 +3232,8 @@
       <c r="N76" s="6"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A77" s="7" t="s">
-        <v>71</v>
+      <c r="A77" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="B77" s="6" t="s">
         <v>20</v>
@@ -3218,17 +3241,21 @@
       <c r="C77" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D77" s="6" t="s">
-        <v>22</v>
+      <c r="D77" s="7" t="s">
+        <v>82</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G77" s="6"/>
-      <c r="H77" s="6"/>
+        <v>26</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G77" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H77" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="I77" s="6"/>
       <c r="J77" s="6"/>
       <c r="K77" s="6"/>
@@ -3238,7 +3265,7 @@
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B78" s="6" t="s">
         <v>20</v>
@@ -3247,23 +3274,21 @@
         <v>19</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F78" s="6" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>3</v>
+        <v>70</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I78" s="6" t="s">
-        <v>34</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I78" s="6"/>
       <c r="J78" s="6"/>
       <c r="K78" s="6"/>
       <c r="L78" s="6"/>
@@ -3272,7 +3297,7 @@
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B79" s="6" t="s">
         <v>20</v>
@@ -3280,23 +3305,23 @@
       <c r="C79" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D79" s="6" t="s">
-        <v>3</v>
+      <c r="D79" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="E79" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F79" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="G79" s="7" t="s">
-        <v>87</v>
+      <c r="F79" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="H79" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I79" s="6" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="J79" s="6"/>
       <c r="K79" s="6"/>
@@ -3306,7 +3331,7 @@
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B80" s="6" t="s">
         <v>20</v>
@@ -3314,23 +3339,23 @@
       <c r="C80" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D80" s="7" t="s">
-        <v>87</v>
+      <c r="D80" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="E80" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F80" s="7" t="s">
-        <v>87</v>
+      <c r="F80" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="H80" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I80" s="6" t="s">
-        <v>88</v>
+        <v>30</v>
       </c>
       <c r="J80" s="6"/>
       <c r="K80" s="6"/>
@@ -3340,7 +3365,7 @@
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B81" s="6" t="s">
         <v>20</v>
@@ -3348,24 +3373,22 @@
       <c r="C81" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D81" s="6" t="s">
-        <v>84</v>
+      <c r="D81" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="E81" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="H81" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I81" s="6" t="s">
-        <v>83</v>
-      </c>
+      <c r="I81" s="6"/>
       <c r="J81" s="6"/>
       <c r="K81" s="6"/>
       <c r="L81" s="6"/>
@@ -3374,7 +3397,7 @@
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B82" s="6" t="s">
         <v>20</v>
@@ -3383,22 +3406,22 @@
         <v>19</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="E82" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F82" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G82" s="7" t="s">
-        <v>89</v>
+        <v>7</v>
+      </c>
+      <c r="G82" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I82" s="6" t="s">
-        <v>88</v>
+      <c r="I82" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="J82" s="6"/>
       <c r="K82" s="6"/>
@@ -3408,7 +3431,7 @@
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B83" s="6" t="s">
         <v>20</v>
@@ -3416,22 +3439,24 @@
       <c r="C83" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D83" s="7" t="s">
-        <v>89</v>
+      <c r="D83" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="E83" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F83" s="7" t="s">
-        <v>89</v>
+      <c r="F83" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I83" s="6"/>
+      <c r="I83" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="J83" s="6"/>
       <c r="K83" s="6"/>
       <c r="L83" s="6"/>
@@ -3440,7 +3465,7 @@
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B84" s="6" t="s">
         <v>20</v>
@@ -3449,21 +3474,23 @@
         <v>19</v>
       </c>
       <c r="D84" s="6" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="E84" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F84" s="6" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="H84" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I84" s="6"/>
+        <v>0</v>
+      </c>
+      <c r="I84" s="6" t="s">
+        <v>88</v>
+      </c>
       <c r="J84" s="6"/>
       <c r="K84" s="6"/>
       <c r="L84" s="6"/>
@@ -3472,31 +3499,31 @@
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G85" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H85" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I85" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="G85" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H85" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I85" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="J85" s="6"/>
       <c r="K85" s="6"/>
@@ -3506,7 +3533,7 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>20</v>
@@ -3515,22 +3542,22 @@
         <v>19</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="E86" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F86" s="6" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I86" s="6" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
@@ -3540,7 +3567,7 @@
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B87" s="6" t="s">
         <v>20</v>
@@ -3548,21 +3575,17 @@
       <c r="C87" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D87" s="7" t="s">
-        <v>15</v>
+      <c r="D87" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F87" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G87" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="H87" s="6" t="s">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
       <c r="I87" s="6"/>
       <c r="J87" s="6"/>
       <c r="K87" s="6"/>
@@ -3572,7 +3595,7 @@
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B88" s="6" t="s">
         <v>20</v>
@@ -3581,22 +3604,22 @@
         <v>19</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E88" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F88" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I88" s="6" t="s">
-        <v>81</v>
+        <v>36</v>
+      </c>
+      <c r="I88" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="J88" s="6"/>
       <c r="K88" s="6"/>
@@ -3606,7 +3629,7 @@
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B89" s="6" t="s">
         <v>20</v>
@@ -3615,23 +3638,17 @@
         <v>19</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="G89" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="H89" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I89" s="6" t="s">
-        <v>83</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
       <c r="J89" s="6"/>
       <c r="K89" s="6"/>
       <c r="L89" s="6"/>
@@ -3640,7 +3657,7 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="6" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>20</v>
@@ -3649,23 +3666,17 @@
         <v>19</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F90" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G90" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H90" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I90" s="6" t="s">
-        <v>96</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
       <c r="J90" s="6"/>
       <c r="K90" s="6"/>
       <c r="L90" s="6"/>
@@ -3674,7 +3685,7 @@
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="6" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>20</v>
@@ -3683,22 +3694,22 @@
         <v>19</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F91" s="6" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="H91" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I91" s="6" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="J91" s="6"/>
       <c r="K91" s="6"/>
@@ -3708,7 +3719,7 @@
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="6" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>20</v>
@@ -3717,23 +3728,21 @@
         <v>19</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="E92" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I92" s="6" t="s">
-        <v>77</v>
-      </c>
+      <c r="I92" s="6"/>
       <c r="J92" s="6"/>
       <c r="K92" s="6"/>
       <c r="L92" s="6"/>
@@ -3742,7 +3751,7 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="6" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>20</v>
@@ -3751,16 +3760,20 @@
         <v>19</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F93" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G93" s="6"/>
-      <c r="H93" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="G93" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="I93" s="6"/>
       <c r="J93" s="6"/>
       <c r="K93" s="6"/>
@@ -3770,7 +3783,7 @@
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B94" s="6" t="s">
         <v>20</v>
@@ -3779,23 +3792,21 @@
         <v>19</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E94" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F94" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I94" s="5" t="s">
-        <v>85</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="I94" s="6"/>
       <c r="J94" s="6"/>
       <c r="K94" s="6"/>
       <c r="L94" s="6"/>
@@ -3804,7 +3815,7 @@
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="6" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B95" s="6" t="s">
         <v>20</v>
@@ -3813,16 +3824,20 @@
         <v>19</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F95" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G95" s="6"/>
-      <c r="H95" s="6"/>
+        <v>93</v>
+      </c>
+      <c r="G95" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H95" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="I95" s="6"/>
       <c r="J95" s="6"/>
       <c r="K95" s="6"/>
@@ -3832,7 +3847,7 @@
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="6" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B96" s="6" t="s">
         <v>20</v>
@@ -3841,16 +3856,20 @@
         <v>19</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F96" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G96" s="6"/>
-      <c r="H96" s="6"/>
+        <v>94</v>
+      </c>
+      <c r="G96" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H96" s="6" t="s">
+        <v>0</v>
+      </c>
       <c r="I96" s="6"/>
       <c r="J96" s="6"/>
       <c r="K96" s="6"/>
@@ -3860,7 +3879,7 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B97" s="6" t="s">
         <v>20</v>
@@ -3869,22 +3888,22 @@
         <v>19</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F97" s="6" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="G97" s="6" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="H97" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I97" s="6" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="J97" s="6"/>
       <c r="K97" s="6"/>
@@ -3894,7 +3913,7 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B98" s="6" t="s">
         <v>20</v>
@@ -3903,21 +3922,23 @@
         <v>19</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="E98" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F98" s="6" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="G98" s="6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="H98" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I98" s="6"/>
+      <c r="I98" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="J98" s="6"/>
       <c r="K98" s="6"/>
       <c r="L98" s="6"/>
@@ -3926,7 +3947,7 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B99" s="6" t="s">
         <v>20</v>
@@ -3935,20 +3956,16 @@
         <v>19</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F99" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G99" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H99" s="6" t="s">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
       <c r="I99" s="6"/>
       <c r="J99" s="6"/>
       <c r="K99" s="6"/>
@@ -3958,7 +3975,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="6" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B100" s="6" t="s">
         <v>20</v>
@@ -3967,20 +3984,16 @@
         <v>19</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E100" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F100" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G100" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="H100" s="6" t="s">
-        <v>0</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
       <c r="I100" s="6"/>
       <c r="J100" s="6"/>
       <c r="K100" s="6"/>
@@ -3990,7 +4003,7 @@
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B101" s="6" t="s">
         <v>20</v>
@@ -3999,21 +4012,23 @@
         <v>19</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>5</v>
+        <v>90</v>
       </c>
       <c r="E101" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F101" s="6" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G101" s="6" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="H101" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I101" s="6"/>
+      <c r="I101" s="6" t="s">
+        <v>96</v>
+      </c>
       <c r="J101" s="6"/>
       <c r="K101" s="6"/>
       <c r="L101" s="6"/>
@@ -4022,30 +4037,32 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E102" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G102" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B102" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C102" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E102" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F102" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="G102" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="H102" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I102" s="6"/>
+      <c r="I102" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="J102" s="6"/>
       <c r="K102" s="6"/>
       <c r="L102" s="6"/>
@@ -4054,32 +4071,30 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D103" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B103" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="E103" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F103" s="6" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="G103" s="6" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="H103" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I103" s="6" t="s">
-        <v>83</v>
-      </c>
+      <c r="I103" s="6"/>
       <c r="J103" s="6"/>
       <c r="K103" s="6"/>
       <c r="L103" s="6"/>
@@ -4088,7 +4103,7 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B104" s="6" t="s">
         <v>20</v>
@@ -4097,32 +4112,32 @@
         <v>19</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="E104" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F104" s="6" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="G104" s="6" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="H104" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I104" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="J104" s="6"/>
-      <c r="K104" s="6"/>
-      <c r="L104" s="6"/>
+      <c r="I104" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="J104" s="5"/>
+      <c r="K104" s="5"/>
+      <c r="L104" s="5"/>
       <c r="M104" s="6"/>
       <c r="N104" s="6"/>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B105" s="6" t="s">
         <v>20</v>
@@ -4131,17 +4146,23 @@
         <v>19</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F105" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G105" s="6"/>
-      <c r="H105" s="6"/>
-      <c r="I105" s="6"/>
+        <v>39</v>
+      </c>
+      <c r="G105" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H105" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I105" s="6" t="s">
+        <v>84</v>
+      </c>
       <c r="J105" s="6"/>
       <c r="K105" s="6"/>
       <c r="L105" s="6"/>
@@ -4150,7 +4171,7 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>20</v>
@@ -4159,26 +4180,32 @@
         <v>19</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F106" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G106" s="6"/>
-      <c r="H106" s="6"/>
-      <c r="I106" s="6"/>
-      <c r="J106" s="6"/>
-      <c r="K106" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="G106" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H106" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I106" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="J106" s="5"/>
+      <c r="K106" s="5"/>
       <c r="L106" s="6"/>
       <c r="M106" s="6"/>
       <c r="N106" s="6"/>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>20</v>
@@ -4187,23 +4214,21 @@
         <v>19</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F107" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>79</v>
+        <v>110</v>
       </c>
       <c r="H107" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I107" s="6" t="s">
-        <v>104</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="I107" s="6"/>
       <c r="J107" s="6"/>
       <c r="K107" s="6"/>
       <c r="L107" s="6"/>
@@ -4212,7 +4237,7 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B108" s="6" t="s">
         <v>20</v>
@@ -4221,22 +4246,22 @@
         <v>19</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="E108" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F108" s="6" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H108" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I108" s="6" t="s">
-        <v>77</v>
+      <c r="I108" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="J108" s="6"/>
       <c r="K108" s="6"/>
@@ -4246,7 +4271,7 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B109" s="6" t="s">
         <v>20</v>
@@ -4255,21 +4280,23 @@
         <v>19</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
       <c r="E109" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F109" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G109" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+      <c r="G109" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="H109" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I109" s="6"/>
+      <c r="I109" s="6" t="s">
+        <v>71</v>
+      </c>
       <c r="J109" s="6"/>
       <c r="K109" s="6"/>
       <c r="L109" s="6"/>
@@ -4278,7 +4305,7 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B110" s="6" t="s">
         <v>20</v>
@@ -4286,33 +4313,33 @@
       <c r="C110" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D110" s="6" t="s">
-        <v>106</v>
+      <c r="D110" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="E110" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F110" s="6" t="s">
-        <v>106</v>
+      <c r="F110" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="H110" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I110" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J110" s="5"/>
-      <c r="K110" s="5"/>
-      <c r="L110" s="5"/>
+        <v>115</v>
+      </c>
+      <c r="J110" s="6"/>
+      <c r="K110" s="6"/>
+      <c r="L110" s="6"/>
       <c r="M110" s="6"/>
       <c r="N110" s="6"/>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B111" s="6" t="s">
         <v>20</v>
@@ -4321,23 +4348,21 @@
         <v>19</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="E111" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F111" s="6" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H111" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I111" s="6" t="s">
-        <v>91</v>
-      </c>
+      <c r="I111" s="6"/>
       <c r="J111" s="6"/>
       <c r="K111" s="6"/>
       <c r="L111" s="6"/>
@@ -4346,7 +4371,7 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B112" s="6" t="s">
         <v>20</v>
@@ -4355,53 +4380,51 @@
         <v>19</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E112" s="6" t="s">
         <v>26</v>
       </c>
       <c r="F112" s="6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I112" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="J112" s="5"/>
-      <c r="K112" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
+      <c r="K112" s="6"/>
       <c r="L112" s="6"/>
       <c r="M112" s="6"/>
       <c r="N112" s="6"/>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B113" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C113" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E113" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F113" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G113" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B113" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C113" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E113" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F113" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="G113" s="6" t="s">
-        <v>118</v>
-      </c>
       <c r="H113" s="6" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="I113" s="6"/>
       <c r="J113" s="6"/>
@@ -4412,7 +4435,7 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B114" s="6" t="s">
         <v>20</v>
@@ -4421,23 +4444,17 @@
         <v>19</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>116</v>
+        <v>10</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F114" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="G114" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="H114" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I114" s="5" t="s">
-        <v>119</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
       <c r="J114" s="6"/>
       <c r="K114" s="6"/>
       <c r="L114" s="6"/>
@@ -4446,41 +4463,30 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="B115" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C115" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D115" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B115" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C115" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>79</v>
-      </c>
       <c r="E115" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="G115" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H115" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I115" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="J115" s="6"/>
-      <c r="K115" s="6"/>
-      <c r="L115" s="6"/>
-      <c r="M115" s="6"/>
-      <c r="N115" s="6"/>
+        <v>103</v>
+      </c>
+      <c r="I115" s="5" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B116" s="6" t="s">
         <v>20</v>
@@ -4488,33 +4494,19 @@
       <c r="C116" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D116" s="8" t="s">
-        <v>7</v>
+      <c r="D116" s="6" t="s">
+        <v>22</v>
       </c>
       <c r="E116" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F116" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G116" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="H116" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I116" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="J116" s="6"/>
-      <c r="K116" s="6"/>
-      <c r="L116" s="6"/>
-      <c r="M116" s="6"/>
-      <c r="N116" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="F116" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A117" s="6" t="s">
-        <v>103</v>
+      <c r="A117" t="s">
+        <v>105</v>
       </c>
       <c r="B117" s="6" t="s">
         <v>20</v>
@@ -4523,122 +4515,110 @@
         <v>19</v>
       </c>
       <c r="D117" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E117" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F117" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G117" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="H117" t="s">
+        <v>0</v>
+      </c>
+      <c r="I117" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>105</v>
       </c>
-      <c r="E117" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F117" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="G117" s="6" t="s">
+      <c r="B118" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C118" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D118" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="E118" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G118" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H118" t="s">
+        <v>0</v>
+      </c>
+      <c r="I118"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>105</v>
+      </c>
+      <c r="B119" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C119" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E119" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G119" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H117" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I117" s="6"/>
-      <c r="J117" s="6"/>
-      <c r="K117" s="6"/>
-      <c r="L117" s="6"/>
-      <c r="M117" s="6"/>
-      <c r="N117" s="6"/>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A118" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B118" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C118" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D118" s="6" t="s">
+      <c r="H119" t="s">
+        <v>0</v>
+      </c>
+      <c r="I119" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>105</v>
+      </c>
+      <c r="B120" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D120" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E118" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F118" s="6" t="s">
+      <c r="E120" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F120" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G118" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="H118" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I118" s="6"/>
-      <c r="J118" s="6"/>
-      <c r="K118" s="6"/>
-      <c r="L118" s="6"/>
-      <c r="M118" s="6"/>
-      <c r="N118" s="6"/>
-    </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A119" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B119" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C119" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E119" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F119" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="G119" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H119" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I119" s="6"/>
-      <c r="J119" s="6"/>
-      <c r="K119" s="6"/>
-      <c r="L119" s="6"/>
-      <c r="M119" s="6"/>
-      <c r="N119" s="6"/>
-    </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A120" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="B120" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C120" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E120" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F120" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G120" s="6"/>
-      <c r="H120" s="6"/>
+      <c r="G120" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="H120" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="I120" s="6"/>
-      <c r="J120" s="6"/>
-      <c r="K120" s="6"/>
-      <c r="L120" s="6"/>
-      <c r="M120" s="6"/>
-      <c r="N120" s="6"/>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A121" s="6" t="s">
-        <v>103</v>
+      <c r="A121" t="s">
+        <v>105</v>
       </c>
       <c r="B121" s="6" t="s">
         <v>20</v>
@@ -4647,21 +4627,27 @@
         <v>19</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="I121" s="5" t="s">
-        <v>112</v>
+        <v>67</v>
+      </c>
+      <c r="G121" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H121" t="s">
+        <v>0</v>
+      </c>
+      <c r="I121" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A122" s="6" t="s">
-        <v>103</v>
+      <c r="A122" t="s">
+        <v>105</v>
       </c>
       <c r="B122" s="6" t="s">
         <v>20</v>
@@ -4670,47 +4656,56 @@
         <v>19</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>22</v>
+        <v>77</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>22</v>
+        <v>77</v>
+      </c>
+      <c r="G122" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="H122" t="s">
+        <v>0</v>
+      </c>
+      <c r="I122" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
+        <v>105</v>
+      </c>
+      <c r="B123" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C123" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E123" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F123" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G123" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H123" t="s">
+        <v>0</v>
+      </c>
+      <c r="I123" s="6" t="s">
         <v>113</v>
-      </c>
-      <c r="B123" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C123" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="E123" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F123" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="G123" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H123" t="s">
-        <v>0</v>
-      </c>
-      <c r="I123" s="6" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B124" s="6" t="s">
         <v>20</v>
@@ -4719,25 +4714,21 @@
         <v>19</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>105</v>
+        <v>10</v>
       </c>
       <c r="E124" s="6" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F124" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="G124" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H124" t="s">
-        <v>0</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G124" s="6"/>
+      <c r="H124"/>
       <c r="I124"/>
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B125" s="6" t="s">
         <v>20</v>
@@ -4746,27 +4737,23 @@
         <v>19</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>42</v>
+        <v>103</v>
       </c>
       <c r="E125" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F125" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G125" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H125" t="s">
-        <v>0</v>
-      </c>
-      <c r="I125" s="6" t="s">
-        <v>91</v>
+        <v>103</v>
+      </c>
+      <c r="G125"/>
+      <c r="H125"/>
+      <c r="I125" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B126" s="6" t="s">
         <v>20</v>
@@ -4775,179 +4762,18 @@
         <v>19</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="E126" s="6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F126" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G126" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="H126" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I126" s="6"/>
-    </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>113</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C127" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D127" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="E127" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F127" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G127" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H127" t="s">
-        <v>0</v>
-      </c>
-      <c r="I127" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>113</v>
-      </c>
-      <c r="B128" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C128" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D128" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E128" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F128" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="G128" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="H128" t="s">
-        <v>0</v>
-      </c>
-      <c r="I128" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>113</v>
-      </c>
-      <c r="B129" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C129" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D129" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="E129" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F129" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="G129" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H129" t="s">
-        <v>0</v>
-      </c>
-      <c r="I129" s="6" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>113</v>
-      </c>
-      <c r="B130" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C130" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E130" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F130" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G130" s="6"/>
-      <c r="H130"/>
-      <c r="I130"/>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>113</v>
-      </c>
-      <c r="B131" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C131" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D131" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="E131" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F131" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G131"/>
-      <c r="H131"/>
-      <c r="I131" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>113</v>
-      </c>
-      <c r="B132" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C132" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D132" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E132" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F132" s="6" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding ozone_aop.py unit process
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksitterl/Documents/Python/watertap3/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E88E76A-A75F-9B41-991C-63EC2B521648}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF36412-2AAD-5242-A86A-A8D1E16F1097}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39600" yWindow="1380" windowWidth="36900" windowHeight="18940" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="42480" yWindow="1760" windowWidth="36900" windowHeight="18940" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1145" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="136">
   <si>
     <t>outlet</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>{"tds_in": 15}</t>
+  </si>
+  <si>
+    <t>ozone_aop</t>
+  </si>
+  <si>
+    <t>{'contact_time': 1, 'ct': 1,'mass_transfer': 0.8, 'aop': False, 'chemical_name': ['Hydrogen_Peroxide']}</t>
   </si>
 </sst>
 </file>
@@ -820,10 +826,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:N140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1141,8 +1147,8 @@
       <c r="F11" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>10</v>
+      <c r="G11" s="4" t="s">
+        <v>134</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>0</v>
@@ -1161,18 +1167,24 @@
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -1181,29 +1193,41 @@
       <c r="B13" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>

</xml_diff>

<commit_message>
edits after kurby/ariel working meeting today 3/4/2021
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksitterl/Documents/Python/watertap3/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFDDE10C-20CB-9D41-9EDF-B9DE8945DBCD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A872F203-6599-034B-A1C2-A6029D3B486D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39560" yWindow="460" windowWidth="36900" windowHeight="20900" activeTab="2" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="840" yWindow="460" windowWidth="36900" windowHeight="20900" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="215">
   <si>
     <t>outlet</t>
   </si>
@@ -678,6 +678,9 @@
   </si>
   <si>
     <t>blackwater</t>
+  </si>
+  <si>
+    <t>{'split_fraction': [0.15, 0.25, 0.6]}</t>
   </si>
 </sst>
 </file>
@@ -1065,10 +1068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
-  <dimension ref="A1:N175"/>
+  <dimension ref="A1:N173"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G151" sqref="G151"/>
+    <sheetView tabSelected="1" topLeftCell="C125" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I143" sqref="I143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2964,23 +2967,19 @@
       <c r="C71" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>22</v>
+      <c r="D71" s="3" t="s">
+        <v>97</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G71" s="2"/>
+        <v>160</v>
+      </c>
       <c r="H71" s="2"/>
-      <c r="I71" s="2"/>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
-      <c r="L71" s="2"/>
-      <c r="M71" s="2"/>
-      <c r="N71" s="2"/>
+      <c r="I71" s="2" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
@@ -2996,50 +2995,60 @@
         <v>97</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>160</v>
+        <v>26</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>176</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A73" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D73" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E73" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F73" s="3" t="s">
-        <v>176</v>
-      </c>
+      <c r="A73" s="2"/>
+      <c r="B73" s="2"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="2"/>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
       <c r="H73" s="2"/>
-      <c r="I73" s="2" t="s">
-        <v>180</v>
-      </c>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+      <c r="M73" s="2"/>
+      <c r="N73" s="2"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="2"/>
-      <c r="E74" s="2"/>
-      <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-      <c r="I74" s="2"/>
+      <c r="A74" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="J74" s="2"/>
       <c r="K74" s="2"/>
       <c r="L74" s="2"/>
@@ -3057,22 +3066,22 @@
         <v>19</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="H75" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="J75" s="2"/>
       <c r="K75" s="2"/>
@@ -3091,23 +3100,21 @@
         <v>19</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="E76" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H76" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I76" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
@@ -3125,21 +3132,23 @@
         <v>19</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="E77" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="H77" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I77" s="2"/>
+      <c r="I77" s="2" t="s">
+        <v>166</v>
+      </c>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
@@ -3157,22 +3166,22 @@
         <v>19</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="E78" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>166</v>
+        <v>109</v>
       </c>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
@@ -3191,22 +3200,22 @@
         <v>19</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="E79" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="H79" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I79" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
@@ -3225,23 +3234,21 @@
         <v>19</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="E80" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="H80" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I80" s="2" t="s">
-        <v>106</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
       <c r="L80" s="2"/>
@@ -3259,21 +3266,23 @@
         <v>19</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H81" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I81" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="J81" s="2"/>
       <c r="K81" s="2"/>
       <c r="L81" s="2"/>
@@ -3291,22 +3300,22 @@
         <v>19</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="E82" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G82" s="2" t="s">
         <v>71</v>
       </c>
+      <c r="G82" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="H82" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>117</v>
+        <v>51</v>
       </c>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
@@ -3324,23 +3333,23 @@
       <c r="C83" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D83" s="2" t="s">
-        <v>52</v>
+      <c r="D83" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E83" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F83" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G83" s="3" t="s">
+      <c r="F83" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="G83" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="H83" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I83" s="2" t="s">
-        <v>51</v>
+        <v>113</v>
       </c>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
@@ -3358,24 +3367,22 @@
       <c r="C84" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D84" s="3" t="s">
-        <v>7</v>
+      <c r="D84" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="E84" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>7</v>
+      <c r="F84" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="H84" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I84" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
       <c r="L84" s="2"/>
@@ -3393,19 +3400,19 @@
         <v>19</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E85" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>80</v>
+        <v>6</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>6</v>
+        <v>78</v>
       </c>
       <c r="H85" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I85" s="2"/>
       <c r="J85" s="2"/>
@@ -3425,19 +3432,19 @@
         <v>19</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="E86" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="H86" s="2" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I86" s="2"/>
       <c r="J86" s="2"/>
@@ -3457,21 +3464,17 @@
         <v>19</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G87" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="H87" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I87" s="2"/>
+      <c r="I87" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="J87" s="2"/>
       <c r="K87" s="2"/>
       <c r="L87" s="2"/>
@@ -3489,17 +3492,17 @@
         <v>19</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>73</v>
+        <v>10</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I88" s="2" t="s">
-        <v>191</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
       <c r="J88" s="2"/>
       <c r="K88" s="2"/>
       <c r="L88" s="2"/>
@@ -3507,24 +3510,12 @@
       <c r="N88" s="2"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A89" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D89" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E89" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F89" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A89" s="2"/>
+      <c r="B89" s="2"/>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -3536,7 +3527,7 @@
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>20</v>
@@ -3545,13 +3536,22 @@
         <v>19</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>22</v>
+        <v>61</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H90" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="J90" s="2"/>
       <c r="K90" s="2"/>
@@ -3560,14 +3560,30 @@
       <c r="N90" s="2"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
-      <c r="E91" s="2"/>
-      <c r="F91" s="2"/>
-      <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
+      <c r="A91" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G91" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H91" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
@@ -3586,22 +3602,22 @@
         <v>19</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="H92" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="J92" s="2"/>
       <c r="K92" s="2"/>
@@ -3620,19 +3636,19 @@
         <v>19</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="E93" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>68</v>
+        <v>6</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="H93" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I93" s="2"/>
       <c r="J93" s="2"/>
@@ -3652,22 +3668,22 @@
         <v>19</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E94" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="H94" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>109</v>
+        <v>163</v>
       </c>
       <c r="J94" s="2"/>
       <c r="K94" s="2"/>
@@ -3686,21 +3702,23 @@
         <v>19</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="E95" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="G95" s="2" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="H95" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I95" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I95" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J95" s="2"/>
       <c r="K95" s="2"/>
       <c r="L95" s="2"/>
@@ -3718,22 +3736,22 @@
         <v>19</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E96" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="H96" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>163</v>
+        <v>81</v>
       </c>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -3752,22 +3770,18 @@
         <v>19</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="G97" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="H97" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
       <c r="I97" s="2" t="s">
-        <v>53</v>
+        <v>191</v>
       </c>
       <c r="J97" s="2"/>
       <c r="K97" s="2"/>
@@ -3786,23 +3800,17 @@
         <v>19</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G98" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H98" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I98" s="2" t="s">
-        <v>81</v>
-      </c>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="I98" s="2"/>
       <c r="J98" s="2"/>
       <c r="K98" s="2"/>
       <c r="L98" s="2"/>
@@ -3820,18 +3828,13 @@
         <v>19</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-      <c r="I99" s="2" t="s">
-        <v>191</v>
+        <v>22</v>
       </c>
       <c r="J99" s="2"/>
       <c r="K99" s="2"/>
@@ -3839,37 +3842,9 @@
       <c r="M99" s="2"/>
       <c r="N99" s="2"/>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A100" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C100" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D100" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E100" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-      <c r="I100" s="2"/>
-      <c r="J100" s="2"/>
-      <c r="K100" s="2"/>
-      <c r="L100" s="2"/>
-      <c r="M100" s="2"/>
-      <c r="N100" s="2"/>
-    </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A101" s="2" t="s">
-        <v>74</v>
+      <c r="A101" s="3" t="s">
+        <v>192</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>20</v>
@@ -3877,20 +3852,53 @@
       <c r="C101" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D101" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E101" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F101" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J101" s="2"/>
-      <c r="K101" s="2"/>
-      <c r="L101" s="2"/>
-      <c r="M101" s="2"/>
-      <c r="N101" s="2"/>
+      <c r="D101" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I101" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E102" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
@@ -3903,22 +3911,22 @@
         <v>19</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>25</v>
+        <v>54</v>
+      </c>
+      <c r="E103" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>196</v>
+        <v>53</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -3938,16 +3946,16 @@
         <v>26</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="H104" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -3961,22 +3969,22 @@
         <v>19</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="E105" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="H105" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I105" s="2" t="s">
-        <v>53</v>
+      <c r="I105" s="3" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
@@ -3990,22 +3998,22 @@
         <v>19</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>97</v>
+        <v>3</v>
       </c>
       <c r="E106" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>96</v>
+        <v>3</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="H106" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I106" s="3" t="s">
-        <v>197</v>
+      <c r="I106" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
@@ -4019,22 +4027,22 @@
         <v>19</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="E107" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>193</v>
+        <v>38</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I107" s="3" t="s">
-        <v>198</v>
+      <c r="I107" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -4048,22 +4056,19 @@
         <v>19</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E108" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="H108" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="I108" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
@@ -4077,22 +4082,19 @@
         <v>19</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="H109" s="3" t="s">
         <v>0</v>
-      </c>
-      <c r="I109" s="2" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -4106,19 +4108,22 @@
         <v>19</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="E110" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
@@ -4132,19 +4137,22 @@
         <v>19</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E111" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="H111" s="3" t="s">
         <v>0</v>
+      </c>
+      <c r="I111" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
@@ -4158,22 +4166,22 @@
         <v>19</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E112" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H112" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
@@ -4186,24 +4194,23 @@
       <c r="C113" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D113" s="3" t="s">
-        <v>7</v>
+      <c r="D113" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H113" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I113" s="2" t="s">
-        <v>113</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G113" s="2"/>
+      <c r="H113" s="2"/>
+      <c r="I113" s="2"/>
+      <c r="J113" s="2"/>
+      <c r="K113" s="2"/>
+      <c r="L113" s="2"/>
+      <c r="M113" s="2"/>
+      <c r="N113" s="2"/>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
@@ -4215,44 +4222,23 @@
       <c r="C114" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D114" s="3" t="s">
-        <v>39</v>
+      <c r="D114" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F114" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G114" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H114" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I114" s="2" t="s">
-        <v>195</v>
+        <v>14</v>
+      </c>
+      <c r="F114" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A115" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C115" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D115" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E115" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F115" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A115" s="2"/>
+      <c r="B115" s="2"/>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2"/>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
@@ -4263,8 +4249,8 @@
       <c r="N115" s="2"/>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A116" s="3" t="s">
-        <v>192</v>
+      <c r="A116" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>20</v>
@@ -4273,25 +4259,57 @@
         <v>19</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>22</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G116" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H116" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
+      <c r="L116" s="2"/>
+      <c r="M116" s="2"/>
+      <c r="N116" s="2"/>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A117" s="2"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="2"/>
-      <c r="E117" s="2"/>
-      <c r="F117" s="2"/>
-      <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
-      <c r="I117" s="2"/>
+      <c r="A117" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D117" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="E117" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F117" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G117" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H117" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>112</v>
+      </c>
       <c r="J117" s="2"/>
       <c r="K117" s="2"/>
       <c r="L117" s="2"/>
@@ -4309,22 +4327,22 @@
         <v>19</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="G118" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H118" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I118" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="J118" s="2"/>
       <c r="K118" s="2"/>
@@ -4343,22 +4361,19 @@
         <v>19</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G119" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H119" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="I119" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="J119" s="2"/>
       <c r="K119" s="2"/>
@@ -4377,22 +4392,22 @@
         <v>19</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E120" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G120" s="2" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="H120" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I120" s="2" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="J120" s="2"/>
       <c r="K120" s="2"/>
@@ -4411,20 +4426,21 @@
         <v>19</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="E121" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>58</v>
+        <v>13</v>
       </c>
       <c r="G121" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="H121" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I121" s="2"/>
       <c r="J121" s="2"/>
       <c r="K121" s="2"/>
       <c r="L121" s="2"/>
@@ -4442,22 +4458,22 @@
         <v>19</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E122" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H122" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
@@ -4476,21 +4492,23 @@
         <v>19</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E123" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="H123" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I123" s="2"/>
+        <v>82</v>
+      </c>
+      <c r="I123" s="2" t="s">
+        <v>214</v>
+      </c>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
@@ -4508,23 +4526,21 @@
         <v>19</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E124" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="G124" s="2" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="H124" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I124" s="2" t="s">
-        <v>109</v>
-      </c>
+      <c r="I124" s="2"/>
       <c r="J124" s="2"/>
       <c r="K124" s="2"/>
       <c r="L124" s="2"/>
@@ -4542,19 +4558,19 @@
         <v>19</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E125" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="G125" s="2" t="s">
-        <v>83</v>
+        <v>39</v>
       </c>
       <c r="H125" s="2" t="s">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="I125" s="2"/>
       <c r="J125" s="2"/>
@@ -4580,7 +4596,7 @@
         <v>26</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>39</v>
@@ -4606,21 +4622,23 @@
         <v>19</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G127" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="H127" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I127" s="2"/>
+      <c r="I127" s="2" t="s">
+        <v>115</v>
+      </c>
       <c r="J127" s="2"/>
       <c r="K127" s="2"/>
       <c r="L127" s="2"/>
@@ -4638,21 +4656,23 @@
         <v>19</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>6</v>
+        <v>43</v>
       </c>
       <c r="E128" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G128" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="H128" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I128" s="2"/>
+      <c r="I128" s="2" t="s">
+        <v>186</v>
+      </c>
       <c r="J128" s="2"/>
       <c r="K128" s="2"/>
       <c r="L128" s="2"/>
@@ -4670,23 +4690,21 @@
         <v>19</v>
       </c>
       <c r="D129" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="G129" s="2" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="H129" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I129" s="2" t="s">
-        <v>115</v>
-      </c>
+      <c r="I129" s="2"/>
       <c r="J129" s="2"/>
       <c r="K129" s="2"/>
       <c r="L129" s="2"/>
@@ -4704,22 +4722,22 @@
         <v>19</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E130" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="G130" s="2" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="H130" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I130" s="2" t="s">
-        <v>186</v>
+        <v>113</v>
       </c>
       <c r="J130" s="2"/>
       <c r="K130" s="2"/>
@@ -4738,21 +4756,23 @@
         <v>19</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E131" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="G131" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H131" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I131" s="2"/>
+      <c r="I131" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="J131" s="2"/>
       <c r="K131" s="2"/>
       <c r="L131" s="2"/>
@@ -4770,22 +4790,22 @@
         <v>19</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G132" s="2" t="s">
-        <v>71</v>
+        <v>13</v>
       </c>
       <c r="H132" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
       <c r="J132" s="2"/>
       <c r="K132" s="2"/>
@@ -4804,23 +4824,17 @@
         <v>19</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G133" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H133" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I133" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="G133" s="2"/>
+      <c r="H133" s="2"/>
+      <c r="I133" s="2"/>
       <c r="J133" s="2"/>
       <c r="K133" s="2"/>
       <c r="L133" s="2"/>
@@ -4838,60 +4852,26 @@
         <v>19</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G134" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H134" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I134" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G134" s="2"/>
+      <c r="H134" s="2"/>
+      <c r="I134" s="2"/>
       <c r="J134" s="2"/>
       <c r="K134" s="2"/>
       <c r="L134" s="2"/>
       <c r="M134" s="2"/>
       <c r="N134" s="2"/>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A135" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B135" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D135" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E135" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F135" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
-      <c r="I135" s="2"/>
-      <c r="J135" s="2"/>
-      <c r="K135" s="2"/>
-      <c r="L135" s="2"/>
-      <c r="M135" s="2"/>
-      <c r="N135" s="2"/>
-    </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A136" s="2" t="s">
-        <v>56</v>
+      <c r="A136" s="3" t="s">
+        <v>200</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>20</v>
@@ -4899,23 +4879,53 @@
       <c r="C136" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D136" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E136" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F136" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
-      <c r="I136" s="2"/>
-      <c r="J136" s="2"/>
-      <c r="K136" s="2"/>
-      <c r="L136" s="2"/>
-      <c r="M136" s="2"/>
-      <c r="N136" s="2"/>
+      <c r="D136" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F136" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I136" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I137" s="2" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
@@ -4928,22 +4938,22 @@
         <v>19</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>25</v>
+        <v>77</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>210</v>
+        <v>77</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>77</v>
+        <v>137</v>
       </c>
       <c r="H138" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I138" s="2" t="s">
-        <v>211</v>
+        <v>117</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
@@ -4957,22 +4967,22 @@
         <v>19</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E139" s="3" t="s">
-        <v>25</v>
+        <v>97</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="F139" s="3" t="s">
-        <v>213</v>
+        <v>137</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="H139" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I139" s="2" t="s">
-        <v>212</v>
+      <c r="I139" s="3" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
@@ -4986,22 +4996,22 @@
         <v>19</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="E140" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>77</v>
+        <v>43</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="H140" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>117</v>
+        <v>186</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
@@ -5015,22 +5025,22 @@
         <v>19</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E141" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>137</v>
+        <v>95</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="H141" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I141" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
@@ -5044,22 +5054,22 @@
         <v>19</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G142" s="3" t="s">
-        <v>95</v>
+        <v>52</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="H142" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I142" s="2" t="s">
-        <v>186</v>
+        <v>205</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
@@ -5073,22 +5083,22 @@
         <v>19</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E143" s="2" t="s">
-        <v>26</v>
+        <v>39</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>95</v>
+        <v>209</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="H143" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I143" s="3" t="s">
-        <v>201</v>
+      <c r="I143" s="2" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
@@ -5102,22 +5112,22 @@
         <v>19</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="E144" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="G144" s="2" t="s">
-        <v>10</v>
+        <v>68</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="H144" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I144" s="2" t="s">
-        <v>205</v>
+        <v>117</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
@@ -5131,22 +5141,22 @@
         <v>19</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>25</v>
+        <v>97</v>
+      </c>
+      <c r="E145" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>209</v>
+        <v>103</v>
       </c>
       <c r="G145" s="3" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="H145" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I145" s="2" t="s">
-        <v>204</v>
+      <c r="I145" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
@@ -5160,22 +5170,22 @@
         <v>19</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="E146" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>68</v>
+        <v>96</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>103</v>
+        <v>207</v>
       </c>
       <c r="H146" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I146" s="2" t="s">
-        <v>117</v>
+      <c r="I146" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
@@ -5189,22 +5199,22 @@
         <v>19</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="E147" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G147" s="3" t="s">
-        <v>96</v>
+        <v>207</v>
+      </c>
+      <c r="G147" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="H147" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I147" s="3" t="s">
-        <v>208</v>
+      <c r="I147" s="2" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
@@ -5217,23 +5227,18 @@
       <c r="C148" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D148" s="3" t="s">
+      <c r="D148" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F148" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G148" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="H148" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F148" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="H148" s="2"/>
       <c r="I148" s="3" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
@@ -5246,24 +5251,16 @@
       <c r="C149" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D149" s="3" t="s">
-        <v>39</v>
+      <c r="D149" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F149" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="G149" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="H149" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I149" s="2" t="s">
-        <v>205</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H149" s="2"/>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
@@ -5276,71 +5273,94 @@
         <v>19</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="H150" s="2"/>
-      <c r="I150" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A151" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B151" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F151" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H151" s="2"/>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A152" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B152" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C152" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E152" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F152" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A152" s="2"/>
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+      <c r="E152" s="2"/>
+      <c r="F152" s="2"/>
+      <c r="G152" s="2"/>
       <c r="H152" s="2"/>
+      <c r="I152" s="2"/>
+      <c r="J152" s="2"/>
+      <c r="K152" s="2"/>
+      <c r="L152" s="2"/>
+      <c r="M152" s="2"/>
+      <c r="N152" s="2"/>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A153" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D153" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E153" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F153" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H153" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I153" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J153" s="2"/>
+      <c r="K153" s="2"/>
+      <c r="L153" s="2"/>
+      <c r="M153" s="2"/>
+      <c r="N153" s="2"/>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A154" s="2"/>
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
-      <c r="D154" s="2"/>
-      <c r="E154" s="2"/>
-      <c r="F154" s="2"/>
-      <c r="G154" s="2"/>
-      <c r="H154" s="2"/>
-      <c r="I154" s="2"/>
+      <c r="A154" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E154" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F154" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G154" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H154" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I154" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
       <c r="L154" s="2"/>
@@ -5358,22 +5378,22 @@
         <v>19</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>1</v>
+        <v>57</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="H155" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I155" s="2" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="J155" s="2"/>
       <c r="K155" s="2"/>
@@ -5392,22 +5412,22 @@
         <v>19</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="H156" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I156" s="2" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="J156" s="2"/>
       <c r="K156" s="2"/>
@@ -5426,22 +5446,22 @@
         <v>19</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E157" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="H157" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I157" s="2" t="s">
-        <v>112</v>
+        <v>165</v>
       </c>
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
@@ -5460,23 +5480,21 @@
         <v>19</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="H158" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I158" s="2" t="s">
-        <v>53</v>
-      </c>
+      <c r="I158" s="2"/>
       <c r="J158" s="2"/>
       <c r="K158" s="2"/>
       <c r="L158" s="2"/>
@@ -5494,23 +5512,21 @@
         <v>19</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H159" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I159" s="2" t="s">
-        <v>165</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I159" s="2"/>
       <c r="J159" s="2"/>
       <c r="K159" s="2"/>
       <c r="L159" s="2"/>
@@ -5528,16 +5544,16 @@
         <v>19</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H160" s="2" t="s">
         <v>0</v>
@@ -5560,21 +5576,23 @@
         <v>19</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E161" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="H161" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I161" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I161" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
       <c r="L161" s="2"/>
@@ -5592,16 +5610,16 @@
         <v>19</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H162" s="2" t="s">
         <v>0</v>
@@ -5624,22 +5642,22 @@
         <v>19</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="H163" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
@@ -5658,21 +5676,23 @@
         <v>19</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="H164" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I164" s="2"/>
+      <c r="I164" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="J164" s="2"/>
       <c r="K164" s="2"/>
       <c r="L164" s="2"/>
@@ -5690,22 +5710,22 @@
         <v>19</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E165" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="G165" s="2" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="H165" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>113</v>
+        <v>163</v>
       </c>
       <c r="J165" s="2"/>
       <c r="K165" s="2"/>
@@ -5724,22 +5744,22 @@
         <v>19</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="E166" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="G166" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H166" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I166" s="2" t="s">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="J166" s="2"/>
       <c r="K166" s="2"/>
@@ -5758,22 +5778,22 @@
         <v>19</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H167" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
       <c r="J167" s="2"/>
       <c r="K167" s="2"/>
@@ -5792,22 +5812,22 @@
         <v>19</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E168" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="I168" s="2" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="J168" s="2"/>
       <c r="K168" s="2"/>
@@ -5826,23 +5846,17 @@
         <v>19</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>52</v>
+        <v>12</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G169" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H169" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I169" s="2" t="s">
-        <v>51</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G169" s="2"/>
+      <c r="H169" s="2"/>
+      <c r="I169" s="2"/>
       <c r="J169" s="2"/>
       <c r="K169" s="2"/>
       <c r="L169" s="2"/>
@@ -5860,23 +5874,17 @@
         <v>19</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G170" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H170" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I170" s="2" t="s">
-        <v>55</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G170" s="2"/>
+      <c r="H170" s="2"/>
+      <c r="I170" s="2"/>
       <c r="J170" s="2"/>
       <c r="K170" s="2"/>
       <c r="L170" s="2"/>
@@ -5894,13 +5902,13 @@
         <v>19</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E171" s="2" t="s">
         <v>14</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="G171" s="2"/>
       <c r="H171" s="2"/>
@@ -5912,80 +5920,24 @@
       <c r="N171" s="2"/>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A172" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D172" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E172" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F172" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G172" s="2"/>
-      <c r="H172" s="2"/>
-      <c r="I172" s="2"/>
-      <c r="J172" s="2"/>
-      <c r="K172" s="2"/>
-      <c r="L172" s="2"/>
-      <c r="M172" s="2"/>
-      <c r="N172" s="2"/>
+      <c r="A172" s="2"/>
+      <c r="B172" s="2"/>
+      <c r="C172" s="2"/>
+      <c r="D172" s="2"/>
+      <c r="E172" s="2"/>
+      <c r="F172" s="2"/>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A173" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D173" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E173" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F173" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G173" s="2"/>
-      <c r="H173" s="2"/>
-      <c r="I173" s="2"/>
-      <c r="J173" s="2"/>
-      <c r="K173" s="2"/>
-      <c r="L173" s="2"/>
-      <c r="M173" s="2"/>
-      <c r="N173" s="2"/>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A174" s="2"/>
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
-      <c r="D174" s="2"/>
-      <c r="E174" s="2"/>
-      <c r="F174" s="2"/>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A175" s="2"/>
-      <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
-      <c r="D175" s="2"/>
-      <c r="E175" s="2"/>
-      <c r="F175" s="2"/>
+      <c r="A173" s="2"/>
+      <c r="B173" s="2"/>
+      <c r="C173" s="2"/>
+      <c r="D173" s="2"/>
+      <c r="E173" s="2"/>
+      <c r="F173" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:I175">
-    <sortCondition ref="A15:A175"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:I173">
+    <sortCondition ref="A15:A173"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5998,7 +5950,7 @@
   <dimension ref="A1:D64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6537,7 +6489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E45408-A136-E347-B0A0-D1652DA1E3C2}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
very small updates to two files
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ksitterl/Documents/Python/watertap3/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3E316E-A9B1-F249-BD5E-1972AF72CED3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1B89E95-654C-0140-9A0F-6E357CD21B3A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="460" windowWidth="36900" windowHeight="20900" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="480" yWindow="460" windowWidth="36900" windowHeight="20900" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1445" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="217">
   <si>
     <t>outlet</t>
   </si>
@@ -683,7 +683,10 @@
     <t>{'split_fraction': [0.15, 0.25, 0.6]}</t>
   </si>
   <si>
-    <t>x</t>
+    <t>{"avg_storage_time": 0.25, 'surge_cap': 0}</t>
+  </si>
+  <si>
+    <t>{"chemical_name": ["Hydrogen_Peroxide"], 'dose': 5, "uv_dose": 100, 'aop': True}</t>
   </si>
 </sst>
 </file>
@@ -1071,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
-  <dimension ref="A1:N173"/>
+  <dimension ref="A1:N172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G64" sqref="G64"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G63" sqref="G63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1617,7 +1620,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>186</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -2779,8 +2782,8 @@
       <c r="F64" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="G64" s="2" t="s">
-        <v>160</v>
+      <c r="G64" s="3" t="s">
+        <v>95</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>0</v>
@@ -2791,7 +2794,7 @@
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>20</v>
@@ -2820,7 +2823,7 @@
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>20</v>
@@ -2846,7 +2849,7 @@
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>20</v>
@@ -2863,7 +2866,7 @@
       <c r="F67" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G67" s="3" t="s">
+      <c r="G67" s="2" t="s">
         <v>178</v>
       </c>
       <c r="H67" s="2" t="s">
@@ -2875,7 +2878,7 @@
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>20</v>
@@ -2904,7 +2907,7 @@
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>20</v>
@@ -2933,7 +2936,7 @@
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>215</v>
+        <v>169</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>20</v>
@@ -2970,7 +2973,7 @@
       <c r="C71" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="2" t="s">
         <v>97</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -2998,7 +3001,7 @@
         <v>97</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>176</v>
@@ -5781,7 +5784,7 @@
         <v>19</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E167" s="2" t="s">
         <v>26</v>
@@ -5796,7 +5799,7 @@
         <v>0</v>
       </c>
       <c r="I167" s="2" t="s">
-        <v>51</v>
+        <v>215</v>
       </c>
       <c r="J167" s="2"/>
       <c r="K167" s="2"/>
@@ -5824,10 +5827,10 @@
         <v>11</v>
       </c>
       <c r="G168" s="2" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="H168" s="2" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="I168" s="2" t="s">
         <v>55</v>
@@ -5849,13 +5852,13 @@
         <v>19</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G169" s="2"/>
       <c r="H169" s="2"/>
@@ -5877,13 +5880,13 @@
         <v>19</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G170" s="2"/>
       <c r="H170" s="2"/>
@@ -5895,32 +5898,12 @@
       <c r="N170" s="2"/>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A171" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D171" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E171" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F171" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G171" s="2"/>
-      <c r="H171" s="2"/>
-      <c r="I171" s="2"/>
-      <c r="J171" s="2"/>
-      <c r="K171" s="2"/>
-      <c r="L171" s="2"/>
-      <c r="M171" s="2"/>
-      <c r="N171" s="2"/>
+      <c r="A171" s="2"/>
+      <c r="B171" s="2"/>
+      <c r="C171" s="2"/>
+      <c r="D171" s="2"/>
+      <c r="E171" s="2"/>
+      <c r="F171" s="2"/>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A172" s="2"/>
@@ -5930,17 +5913,9 @@
       <c r="E172" s="2"/>
       <c r="F172" s="2"/>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A173" s="2"/>
-      <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
-      <c r="D173" s="2"/>
-      <c r="E173" s="2"/>
-      <c r="F173" s="2"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:I173">
-    <sortCondition ref="A15:A173"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:I172">
+    <sortCondition ref="A15:A172"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished splitter option. assumes even split unless specifiedd in parameters. there is an option to optimize the split stream
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF0E607-0EEF-BC41-B5EC-CA5F120FDF7D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC070684-5766-C345-AA7F-3DB49D88FD79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6560" yWindow="10860" windowWidth="45140" windowHeight="26500" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="760" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="225">
   <si>
     <t>outlet</t>
   </si>
@@ -584,9 +584,6 @@
     <t>{"chemical_name": ["Hydrogen_Peroxide"], 'dose': 5, "uv_dose": 80, 'aop': True}</t>
   </si>
   <si>
-    <t>{"unit_process_name": 'microfiltration'}</t>
-  </si>
-  <si>
     <t>ro_deep,uv_aop</t>
   </si>
   <si>
@@ -699,6 +696,21 @@
   </si>
   <si>
     <t>Santa_Barbara_x</t>
+  </si>
+  <si>
+    <t>{"unit_process_name": 'microfiltration', "split_fraction": [0.4, 0.6]}</t>
+  </si>
+  <si>
+    <t>ANY</t>
+  </si>
+  <si>
+    <t>{"split_faction": [X, X, X]}</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>if the stream is split, the specify split, the number of outlets needs to match length of split list</t>
   </si>
 </sst>
 </file>
@@ -1102,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E126" sqref="E126"/>
+    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1114,7 +1126,7 @@
     <col min="4" max="4" width="30.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="20.33203125" style="3" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="57.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48" style="3" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" style="3" customWidth="1"/>
     <col min="9" max="9" width="98.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="10.83203125" style="3"/>
@@ -1311,7 +1323,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>35</v>
@@ -1329,13 +1341,13 @@
         <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>7</v>
@@ -1562,7 +1574,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1585,13 +1597,13 @@
         <v>91</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>163</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>182</v>
+        <v>220</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1620,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1649,7 +1661,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1678,7 +1690,7 @@
         <v>0</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1943,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -2051,7 +2063,7 @@
         <v>5</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>0</v>
@@ -2075,16 +2087,16 @@
         <v>26</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -2104,7 +2116,7 @@
         <v>26</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>7</v>
@@ -2113,7 +2125,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2821,7 +2833,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -3482,7 +3494,7 @@
         <v>70</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
@@ -3620,7 +3632,7 @@
         <v>38</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>0</v>
@@ -3645,13 +3657,13 @@
         <v>19</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>73</v>
@@ -3790,7 +3802,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -3853,7 +3865,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>20</v>
@@ -3877,12 +3889,12 @@
         <v>0</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>20</v>
@@ -3906,12 +3918,12 @@
         <v>0</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>20</v>
@@ -3940,7 +3952,7 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>20</v>
@@ -3958,18 +3970,18 @@
         <v>91</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>20</v>
@@ -3984,7 +3996,7 @@
         <v>26</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G104" s="3" t="s">
         <v>3</v>
@@ -3993,12 +4005,12 @@
         <v>0</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>20</v>
@@ -4027,7 +4039,7 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>20</v>
@@ -4056,7 +4068,7 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>20</v>
@@ -4082,7 +4094,7 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>20</v>
@@ -4108,7 +4120,7 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>20</v>
@@ -4137,7 +4149,7 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>20</v>
@@ -4166,7 +4178,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>20</v>
@@ -4190,12 +4202,12 @@
         <v>0</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>20</v>
@@ -4223,7 +4235,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>20</v>
@@ -4327,7 +4339,7 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>20</v>
@@ -4361,7 +4373,7 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>20</v>
@@ -4392,7 +4404,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>20</v>
@@ -4426,7 +4438,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>20</v>
@@ -4458,7 +4470,7 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>20</v>
@@ -4492,7 +4504,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>20</v>
@@ -4516,7 +4528,7 @@
         <v>0</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
@@ -4526,7 +4538,7 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>20</v>
@@ -4550,7 +4562,7 @@
         <v>0</v>
       </c>
       <c r="I123" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
@@ -4560,7 +4572,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>20</v>
@@ -4594,7 +4606,7 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>20</v>
@@ -4628,7 +4640,7 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>20</v>
@@ -4660,7 +4672,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>20</v>
@@ -4694,7 +4706,7 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>20</v>
@@ -4728,7 +4740,7 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>20</v>
@@ -4760,7 +4772,7 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>20</v>
@@ -4816,7 +4828,7 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>20</v>
@@ -4844,7 +4856,7 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>20</v>
@@ -4859,7 +4871,7 @@
         <v>25</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>74</v>
@@ -4868,12 +4880,12 @@
         <v>0</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B135" s="2" t="s">
         <v>20</v>
@@ -4888,7 +4900,7 @@
         <v>25</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G135" s="3" t="s">
         <v>74</v>
@@ -4897,12 +4909,12 @@
         <v>0</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>20</v>
@@ -4931,7 +4943,7 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>20</v>
@@ -4955,12 +4967,12 @@
         <v>0</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B138" s="2" t="s">
         <v>20</v>
@@ -4989,7 +5001,7 @@
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B139" s="2" t="s">
         <v>20</v>
@@ -5013,12 +5025,12 @@
         <v>0</v>
       </c>
       <c r="I139" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="140" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B140" s="2" t="s">
         <v>20</v>
@@ -5042,12 +5054,12 @@
         <v>0</v>
       </c>
       <c r="I140" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B141" s="2" t="s">
         <v>20</v>
@@ -5062,7 +5074,7 @@
         <v>25</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G141" s="3" t="s">
         <v>65</v>
@@ -5071,12 +5083,12 @@
         <v>0</v>
       </c>
       <c r="I141" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B142" s="2" t="s">
         <v>20</v>
@@ -5105,7 +5117,7 @@
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>20</v>
@@ -5129,12 +5141,12 @@
         <v>0</v>
       </c>
       <c r="I143" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>20</v>
@@ -5152,18 +5164,18 @@
         <v>91</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H144" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I144" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>20</v>
@@ -5178,21 +5190,21 @@
         <v>26</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G145" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H145" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I145" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>20</v>
@@ -5207,16 +5219,16 @@
         <v>27</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H146" s="2"/>
       <c r="I146" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B147" s="2" t="s">
         <v>20</v>
@@ -5237,7 +5249,7 @@
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B148" s="2" t="s">
         <v>20</v>
@@ -5766,7 +5778,7 @@
         <v>0</v>
       </c>
       <c r="I165" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J165" s="2"/>
       <c r="K165" s="2"/>
@@ -5892,17 +5904,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586A0CBC-F2B8-8D43-BF36-A9434BF68145}">
-  <dimension ref="A1:D64"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="142.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="73.6640625" style="5" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="5"/>
     <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -5923,134 +5935,137 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>221</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>103</v>
+        <v>222</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>100</v>
+        <v>223</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>100</v>
+        <v>116</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>104</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>127</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>158</v>
+        <v>84</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>100</v>
+        <v>116</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B12" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C12" s="5" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>85</v>
@@ -6060,88 +6075,88 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>179</v>
+      <c r="A14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>161</v>
+        <v>179</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>100</v>
@@ -6149,281 +6164,292 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>29</v>
+        <v>99</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>126</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B25" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D25" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="6" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
-      <c r="B26" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="B27" s="2" t="s">
-        <v>197</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="2" t="s">
-        <v>96</v>
+        <v>196</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="2" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="2" t="s">
-        <v>188</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="2" t="s">
-        <v>98</v>
+        <v>187</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="2" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="2" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="2" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="B38" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="2" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="2" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="2" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="2" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="2" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
       <c r="B50" s="2" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="B52" s="2" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
       <c r="B53" s="2" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
       <c r="B54" s="2" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
       <c r="B55" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
       <c r="B56" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
       <c r="B57" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
       <c r="B58" s="2" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
       <c r="B59" s="2" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="6"/>
       <c r="B60" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="6"/>
+      <c r="B61" s="2" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B61" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B62" s="2" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D24">
-    <sortCondition ref="A1:A24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D25">
+    <sortCondition ref="A1:A25"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updates to excel and csvs to run with RO deep changes
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC070684-5766-C345-AA7F-3DB49D88FD79}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A8FBFE-323A-444D-8ECA-242351D1D3E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="460" windowWidth="28800" windowHeight="16320" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="10740" yWindow="4980" windowWidth="28800" windowHeight="16320" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -692,9 +692,6 @@
     <t>{"alum_dose" : 0.0, "polymer_dose": 0.0}</t>
   </si>
   <si>
-    <t>{"pass": "first", "membrane_area": 500000, "feed_pressure": 65}</t>
-  </si>
-  <si>
     <t>Santa_Barbara_x</t>
   </si>
   <si>
@@ -711,6 +708,9 @@
   </si>
   <si>
     <t>if the stream is split, the specify split, the number of outlets needs to match length of split list</t>
+  </si>
+  <si>
+    <t>{"pass": "first", "membrane_area": 50000, "feed_pressure": 65}</t>
   </si>
 </sst>
 </file>
@@ -1114,8 +1114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1603,7 +1603,7 @@
         <v>163</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1622,7 +1622,7 @@
       <c r="E19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="3" t="s">
@@ -1632,7 +1632,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -4339,7 +4339,7 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>20</v>
@@ -4373,7 +4373,7 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>20</v>
@@ -4404,7 +4404,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>20</v>
@@ -4438,7 +4438,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>20</v>
@@ -4470,7 +4470,7 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>20</v>
@@ -4504,7 +4504,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>20</v>
@@ -4538,7 +4538,7 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>20</v>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>20</v>
@@ -4606,7 +4606,7 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>20</v>
@@ -4640,7 +4640,7 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>20</v>
@@ -4672,7 +4672,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>20</v>
@@ -4706,7 +4706,7 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>20</v>
@@ -4740,7 +4740,7 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>20</v>
@@ -4772,7 +4772,7 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>20</v>
@@ -4828,7 +4828,7 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>20</v>
@@ -5907,7 +5907,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5935,16 +5935,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
cleaning files and updating ro deep
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A8FBFE-323A-444D-8ECA-242351D1D3E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9019E1-E224-FC4C-80A7-1D8723BAD505}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10740" yWindow="4980" windowWidth="28800" windowHeight="16320" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="10540" yWindow="1620" windowWidth="35640" windowHeight="23220" activeTab="1" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="227">
   <si>
     <t>outlet</t>
   </si>
@@ -590,9 +590,6 @@
     <t>{"avg_storage_time": 0.25, 'surge_cap': 0.0000001}</t>
   </si>
   <si>
-    <t>{"source_type": ["Big_Spring_Feed"], "avg_storage_time": 0.25, 'surge_cap': 0}</t>
-  </si>
-  <si>
     <t>{"incl_piping": False, "pipe_distance": 22}</t>
   </si>
   <si>
@@ -632,36 +629,15 @@
     <t>{'unit_process_name': 'mbr_nitrification'}</t>
   </si>
   <si>
-    <t>{"source_type": ["Solaire_Stormwater"], "avg_storage_time": 1, 'surge_cap': 0.2}</t>
-  </si>
-  <si>
     <t>{"avg_storage_time": 0.125, 'surge_cap': 0.2}</t>
   </si>
   <si>
     <t>{'unit_process_name': 'agriculture'}</t>
   </si>
   <si>
-    <t>treated_storage_2</t>
-  </si>
-  <si>
     <t>{'unit_process_name': 'cas'}</t>
   </si>
   <si>
-    <t>stormwater</t>
-  </si>
-  <si>
-    <t>graywater</t>
-  </si>
-  <si>
-    <t>{"source_type": ["Solaire_Graywater"], "avg_storage_time": 1, 'surge_cap': 0.2}</t>
-  </si>
-  <si>
-    <t>{"source_type": ["Solaire_Blackwater"], "avg_storage_time": 1, 'surge_cap': 0.2}</t>
-  </si>
-  <si>
-    <t>blackwater</t>
-  </si>
-  <si>
     <t>{'split_fraction': [0.15, 0.25, 0.6]}</t>
   </si>
   <si>
@@ -711,6 +687,36 @@
   </si>
   <si>
     <t>{"pass": "first", "membrane_area": 50000, "feed_pressure": 65}</t>
+  </si>
+  <si>
+    <t>stormwater_tank</t>
+  </si>
+  <si>
+    <t>{"water_type": ["Solaire_Graywater", "Solaire_Blackwater"], "avg_storage_time": 1, 'surge_cap': 0.2}</t>
+  </si>
+  <si>
+    <t>{"water_type": ["Solaire_Stormwater"], "avg_storage_time": 1, 'surge_cap': 0.2}</t>
+  </si>
+  <si>
+    <t>gray_and_black_tank</t>
+  </si>
+  <si>
+    <t>{"water_type": ["Seawater"]}</t>
+  </si>
+  <si>
+    <t>agriculture,municipal_drinking</t>
+  </si>
+  <si>
+    <t>{"water_type": ["Big_Spring_Feed"], "avg_storage_time": 0.25, 'surge_cap': 0}</t>
+  </si>
+  <si>
+    <t>Big_Spring_x</t>
+  </si>
+  <si>
+    <t>{"pass": "first" or "second", "feed_pressure": value}</t>
+  </si>
+  <si>
+    <t>bar for pressure</t>
   </si>
 </sst>
 </file>
@@ -1112,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
-  <dimension ref="A1:N170"/>
+  <dimension ref="A1:N168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1323,7 +1329,7 @@
         <v>13</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>35</v>
@@ -1341,13 +1347,13 @@
         <v>19</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>7</v>
@@ -1574,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>184</v>
+        <v>223</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1603,7 +1609,7 @@
         <v>163</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1632,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1661,7 +1667,7 @@
         <v>0</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1715,7 +1721,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>178</v>
+        <v>224</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>20</v>
@@ -1926,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>31</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1955,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -2063,7 +2069,7 @@
         <v>5</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>0</v>
@@ -2087,16 +2093,16 @@
         <v>26</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -2116,7 +2122,7 @@
         <v>26</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>7</v>
@@ -2125,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -2833,7 +2839,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -3494,7 +3500,7 @@
         <v>70</v>
       </c>
       <c r="I86" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
@@ -3632,7 +3638,7 @@
         <v>38</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>0</v>
@@ -3657,13 +3663,13 @@
         <v>19</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>73</v>
@@ -3802,7 +3808,7 @@
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J96" s="2"/>
       <c r="K96" s="2"/>
@@ -3865,7 +3871,7 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>20</v>
@@ -3889,12 +3895,12 @@
         <v>0</v>
       </c>
       <c r="I100" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>20</v>
@@ -3918,12 +3924,12 @@
         <v>0</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>20</v>
@@ -3952,7 +3958,7 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>20</v>
@@ -3970,18 +3976,18 @@
         <v>91</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H103" s="3" t="s">
         <v>0</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>20</v>
@@ -3996,7 +4002,7 @@
         <v>26</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G104" s="3" t="s">
         <v>3</v>
@@ -4005,12 +4011,12 @@
         <v>0</v>
       </c>
       <c r="I104" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>20</v>
@@ -4039,7 +4045,7 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>20</v>
@@ -4068,7 +4074,7 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>20</v>
@@ -4094,7 +4100,7 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>20</v>
@@ -4120,7 +4126,7 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B109" s="2" t="s">
         <v>20</v>
@@ -4149,7 +4155,7 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>20</v>
@@ -4178,7 +4184,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>20</v>
@@ -4202,12 +4208,12 @@
         <v>0</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>20</v>
@@ -4235,7 +4241,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>20</v>
@@ -4339,7 +4345,7 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>20</v>
@@ -4373,7 +4379,7 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>20</v>
@@ -4404,7 +4410,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>20</v>
@@ -4438,7 +4444,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>20</v>
@@ -4470,7 +4476,7 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>20</v>
@@ -4504,7 +4510,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>20</v>
@@ -4528,7 +4534,7 @@
         <v>0</v>
       </c>
       <c r="I122" s="2" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="J122" s="2"/>
       <c r="K122" s="2"/>
@@ -4538,7 +4544,7 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>20</v>
@@ -4562,7 +4568,7 @@
         <v>0</v>
       </c>
       <c r="I123" s="8" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="J123" s="2"/>
       <c r="K123" s="2"/>
@@ -4572,7 +4578,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>20</v>
@@ -4606,7 +4612,7 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>20</v>
@@ -4640,7 +4646,7 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>20</v>
@@ -4672,7 +4678,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>20</v>
@@ -4706,7 +4712,7 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>20</v>
@@ -4740,7 +4746,7 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>20</v>
@@ -4772,7 +4778,7 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>20</v>
@@ -4828,7 +4834,7 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>20</v>
@@ -4856,7 +4862,7 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B134" s="2" t="s">
         <v>20</v>
@@ -4871,7 +4877,7 @@
         <v>25</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>74</v>
@@ -4880,244 +4886,254 @@
         <v>0</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>205</v>
+        <v>218</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A135" s="3" t="s">
+      <c r="A135" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D135" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F135" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H135" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I135" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="J135" s="2"/>
+      <c r="K135" s="2"/>
+      <c r="L135" s="2"/>
+      <c r="M135" s="2"/>
+      <c r="N135" s="2"/>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A136" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I136" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="J136" s="2"/>
+      <c r="K136" s="2"/>
+      <c r="L136" s="2"/>
+      <c r="M136" s="2"/>
+      <c r="N136" s="2"/>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A137" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F137" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G137" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="H137" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I137" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A138" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F138" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H138" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A139" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F139" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="H139" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I139" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A140" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B140" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C140" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F140" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H140" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I140" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B135" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D135" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E135" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F135" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="G135" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="H135" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I135" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A136" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B136" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D136" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E136" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F136" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G136" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H136" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I136" s="2" t="s">
+    </row>
+    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A141" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B141" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C141" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F141" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G141" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H141" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I141" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A137" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D137" s="3" t="s">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A142" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D142" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="E137" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F137" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="G137" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="H137" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I137" s="3" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A138" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D138" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E138" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F138" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G138" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="H138" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I138" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A139" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D139" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E139" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F139" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G139" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H139" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I139" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A140" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D140" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E140" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F140" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G140" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H140" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I140" s="2" t="s">
+      <c r="E142" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F142" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I142" s="3" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A141" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B141" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D141" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="E141" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F141" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="G141" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H141" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I141" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A142" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B142" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D142" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E142" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F142" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G142" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="H142" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I142" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A143" s="3" t="s">
-        <v>194</v>
+      <c r="A143" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="B143" s="2" t="s">
         <v>20</v>
@@ -5132,21 +5148,21 @@
         <v>26</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G143" s="3" t="s">
         <v>91</v>
       </c>
+      <c r="G143" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="H143" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I143" s="3" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A144" s="3" t="s">
-        <v>194</v>
+      <c r="A144" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="B144" s="2" t="s">
         <v>20</v>
@@ -5154,28 +5170,23 @@
       <c r="C144" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D144" s="3" t="s">
+      <c r="D144" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F144" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G144" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H144" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F144" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="H144" s="2"/>
       <c r="I144" s="3" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A145" s="3" t="s">
-        <v>194</v>
+      <c r="A145" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="B145" s="2" t="s">
         <v>20</v>
@@ -5183,28 +5194,20 @@
       <c r="C145" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D145" s="3" t="s">
-        <v>39</v>
+      <c r="D145" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F145" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="G145" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="H145" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I145" s="2" t="s">
-        <v>199</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="F145" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H145" s="2"/>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A146" s="3" t="s">
-        <v>194</v>
+      <c r="A146" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="B146" s="2" t="s">
         <v>20</v>
@@ -5213,71 +5216,94 @@
         <v>19</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>196</v>
+        <v>22</v>
       </c>
       <c r="H146" s="2"/>
-      <c r="I146" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A147" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E147" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F147" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H147" s="2"/>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A148" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E148" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F148" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A148" s="2"/>
+      <c r="B148" s="2"/>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+      <c r="E148" s="2"/>
+      <c r="F148" s="2"/>
+      <c r="G148" s="2"/>
       <c r="H148" s="2"/>
+      <c r="I148" s="2"/>
+      <c r="J148" s="2"/>
+      <c r="K148" s="2"/>
+      <c r="L148" s="2"/>
+      <c r="M148" s="2"/>
+      <c r="N148" s="2"/>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A149" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I149" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J149" s="2"/>
+      <c r="K149" s="2"/>
+      <c r="L149" s="2"/>
+      <c r="M149" s="2"/>
+      <c r="N149" s="2"/>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A150" s="2"/>
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
-      <c r="D150" s="2"/>
-      <c r="E150" s="2"/>
-      <c r="F150" s="2"/>
-      <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
-      <c r="I150" s="2"/>
+      <c r="A150" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E150" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F150" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H150" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I150" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="J150" s="2"/>
       <c r="K150" s="2"/>
       <c r="L150" s="2"/>
@@ -5295,22 +5321,22 @@
         <v>19</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="H151" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I151" s="2" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="J151" s="2"/>
       <c r="K151" s="2"/>
@@ -5329,22 +5355,22 @@
         <v>19</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="E152" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="G152" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H152" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I152" s="2" t="s">
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="J152" s="2"/>
       <c r="K152" s="2"/>
@@ -5363,22 +5389,22 @@
         <v>19</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="E153" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G153" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="H153" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I153" s="2" t="s">
-        <v>107</v>
+        <v>160</v>
       </c>
       <c r="J153" s="2"/>
       <c r="K153" s="2"/>
@@ -5397,23 +5423,21 @@
         <v>19</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E154" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G154" s="2" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="H154" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I154" s="2" t="s">
-        <v>50</v>
-      </c>
+      <c r="I154" s="2"/>
       <c r="J154" s="2"/>
       <c r="K154" s="2"/>
       <c r="L154" s="2"/>
@@ -5431,23 +5455,21 @@
         <v>19</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="E155" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="H155" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I155" s="2" t="s">
-        <v>160</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I155" s="2"/>
       <c r="J155" s="2"/>
       <c r="K155" s="2"/>
       <c r="L155" s="2"/>
@@ -5465,16 +5487,16 @@
         <v>19</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="E156" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="G156" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="H156" s="2" t="s">
         <v>0</v>
@@ -5497,21 +5519,23 @@
         <v>19</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E157" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G157" s="2" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="H157" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I157" s="2"/>
+        <v>0</v>
+      </c>
+      <c r="I157" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="J157" s="2"/>
       <c r="K157" s="2"/>
       <c r="L157" s="2"/>
@@ -5529,16 +5553,16 @@
         <v>19</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E158" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G158" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H158" s="2" t="s">
         <v>0</v>
@@ -5561,22 +5585,22 @@
         <v>19</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E159" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="H159" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I159" s="2" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="J159" s="2"/>
       <c r="K159" s="2"/>
@@ -5595,21 +5619,23 @@
         <v>19</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="E160" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>15</v>
+        <v>56</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="H160" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I160" s="2"/>
+      <c r="I160" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="J160" s="2"/>
       <c r="K160" s="2"/>
       <c r="L160" s="2"/>
@@ -5627,22 +5653,22 @@
         <v>19</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="E161" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="G161" s="2" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="H161" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I161" s="2" t="s">
-        <v>108</v>
+        <v>158</v>
       </c>
       <c r="J161" s="2"/>
       <c r="K161" s="2"/>
@@ -5661,22 +5687,22 @@
         <v>19</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>51</v>
+        <v>9</v>
       </c>
       <c r="E162" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="G162" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H162" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I162" s="2" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="J162" s="2"/>
       <c r="K162" s="2"/>
@@ -5695,22 +5721,22 @@
         <v>19</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E163" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H163" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I163" s="2" t="s">
-        <v>158</v>
+        <v>201</v>
       </c>
       <c r="J163" s="2"/>
       <c r="K163" s="2"/>
@@ -5729,22 +5755,22 @@
         <v>19</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E164" s="2" t="s">
         <v>26</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G164" s="2" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="H164" s="2" t="s">
         <v>0</v>
       </c>
       <c r="I164" s="2" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="J164" s="2"/>
       <c r="K164" s="2"/>
@@ -5763,23 +5789,17 @@
         <v>19</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G165" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H165" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I165" s="2" t="s">
-        <v>209</v>
-      </c>
+      <c r="G165" s="2"/>
+      <c r="H165" s="2"/>
+      <c r="I165" s="2"/>
       <c r="J165" s="2"/>
       <c r="K165" s="2"/>
       <c r="L165" s="2"/>
@@ -5797,23 +5817,17 @@
         <v>19</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G166" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H166" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="I166" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="G166" s="2"/>
+      <c r="H166" s="2"/>
+      <c r="I166" s="2"/>
       <c r="J166" s="2"/>
       <c r="K166" s="2"/>
       <c r="L166" s="2"/>
@@ -5821,80 +5835,24 @@
       <c r="N166" s="2"/>
     </row>
     <row r="167" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A167" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C167" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E167" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F167" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G167" s="2"/>
-      <c r="H167" s="2"/>
-      <c r="I167" s="2"/>
-      <c r="J167" s="2"/>
-      <c r="K167" s="2"/>
-      <c r="L167" s="2"/>
-      <c r="M167" s="2"/>
-      <c r="N167" s="2"/>
+      <c r="A167" s="2"/>
+      <c r="B167" s="2"/>
+      <c r="C167" s="2"/>
+      <c r="D167" s="2"/>
+      <c r="E167" s="2"/>
+      <c r="F167" s="2"/>
     </row>
     <row r="168" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A168" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E168" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F168" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G168" s="2"/>
-      <c r="H168" s="2"/>
-      <c r="I168" s="2"/>
-      <c r="J168" s="2"/>
-      <c r="K168" s="2"/>
-      <c r="L168" s="2"/>
-      <c r="M168" s="2"/>
-      <c r="N168" s="2"/>
-    </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A169" s="2"/>
-      <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
-      <c r="D169" s="2"/>
-      <c r="E169" s="2"/>
-      <c r="F169" s="2"/>
-    </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A170" s="2"/>
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
-      <c r="D170" s="2"/>
-      <c r="E170" s="2"/>
-      <c r="F170" s="2"/>
+      <c r="A168" s="2"/>
+      <c r="B168" s="2"/>
+      <c r="C168" s="2"/>
+      <c r="D168" s="2"/>
+      <c r="E168" s="2"/>
+      <c r="F168" s="2"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:I170">
-    <sortCondition ref="A15:A170"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A15:I168">
+    <sortCondition ref="A15:A168"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5904,10 +5862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586A0CBC-F2B8-8D43-BF36-A9434BF68145}">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5935,148 +5893,148 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>103</v>
+        <v>225</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>100</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>100</v>
+        <v>116</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>52</v>
+        <v>104</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>127</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>158</v>
+        <v>84</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>100</v>
+        <v>116</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C13" s="5" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>85</v>
@@ -6086,88 +6044,88 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>179</v>
+      <c r="A15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>161</v>
+        <v>179</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B19" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>167</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>100</v>
@@ -6175,281 +6133,292 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>99</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>126</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C26" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D26" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="6" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="6"/>
-      <c r="B27" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="6"/>
       <c r="B28" s="2" t="s">
-        <v>196</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="2" t="s">
-        <v>96</v>
+        <v>195</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="2" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="2" t="s">
-        <v>187</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="2" t="s">
-        <v>98</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="2" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="2" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="B38" s="2" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="2" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="2" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="2" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="2" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
       <c r="B50" s="2" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="2" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="B52" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
       <c r="B53" s="2" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
       <c r="B54" s="2" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
       <c r="B55" s="2" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
       <c r="B56" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
       <c r="B57" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
       <c r="B58" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
       <c r="B59" s="2" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="6"/>
       <c r="B60" s="2" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
       <c r="B61" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="6"/>
+      <c r="B62" s="2" t="s">
         <v>149</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B62" s="2" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B63" s="2" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B64" s="2" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="s">
         <v>141</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:D25">
-    <sortCondition ref="A1:A25"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D26">
+    <sortCondition ref="A1:A26"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixing coag and floc bug, adding values to train inputs
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9019E1-E224-FC4C-80A7-1D8723BAD505}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DFA211-A795-8044-8B86-03A9025DE76D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="1620" windowWidth="35640" windowHeight="23220" activeTab="1" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="10540" yWindow="1620" windowWidth="35640" windowHeight="23220" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -665,9 +665,6 @@
     <t>{"pass": "second", "membrane_area": 500000, "feed_pressure": 40}</t>
   </si>
   <si>
-    <t>{"alum_dose" : 0.0, "polymer_dose": 0.0}</t>
-  </si>
-  <si>
     <t>Santa_Barbara_x</t>
   </si>
   <si>
@@ -717,6 +714,9 @@
   </si>
   <si>
     <t>bar for pressure</t>
+  </si>
+  <si>
+    <t>{"alum_dose" : 10, "polymer_dose": 0.1}</t>
   </si>
 </sst>
 </file>
@@ -1120,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:N168"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1580,7 +1580,7 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
@@ -1609,7 +1609,7 @@
         <v>163</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
@@ -1638,7 +1638,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1721,7 +1721,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>20</v>
@@ -1932,7 +1932,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
@@ -1961,7 +1961,7 @@
         <v>0</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
@@ -4345,7 +4345,7 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>20</v>
@@ -4379,7 +4379,7 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>20</v>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>20</v>
@@ -4444,7 +4444,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>20</v>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>20</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>20</v>
@@ -4544,7 +4544,7 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>20</v>
@@ -4578,7 +4578,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>20</v>
@@ -4612,7 +4612,7 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>20</v>
@@ -4646,7 +4646,7 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>20</v>
@@ -4678,7 +4678,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>20</v>
@@ -4712,7 +4712,7 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>20</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>20</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>20</v>
@@ -4834,7 +4834,7 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>20</v>
@@ -4877,7 +4877,7 @@
         <v>25</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>74</v>
@@ -4886,7 +4886,7 @@
         <v>0</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
@@ -4906,7 +4906,7 @@
         <v>25</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>65</v>
@@ -4915,7 +4915,7 @@
         <v>0</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
@@ -4943,7 +4943,7 @@
         <v>49</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>163</v>
@@ -5864,7 +5864,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586A0CBC-F2B8-8D43-BF36-A9434BF68145}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -5893,16 +5893,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5910,10 +5910,10 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>225</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updating reverse osmosis to handle stages. updating files to read in new csvs.
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DFA211-A795-8044-8B86-03A9025DE76D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59E41A7-3F4A-9C4B-A60E-F0BA7A317F49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10540" yWindow="1620" windowWidth="35640" windowHeight="23220" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="13520" yWindow="1740" windowWidth="35640" windowHeight="23220" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1413" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="232">
   <si>
     <t>outlet</t>
   </si>
@@ -662,18 +662,12 @@
     <t>{"pass": "first", "membrane_area": 500000, "feed_pressure": 90}</t>
   </si>
   <si>
-    <t>{"pass": "second", "membrane_area": 500000, "feed_pressure": 40}</t>
-  </si>
-  <si>
     <t>Santa_Barbara_x</t>
   </si>
   <si>
     <t>{"unit_process_name": 'microfiltration', "split_fraction": [0.4, 0.6]}</t>
   </si>
   <si>
-    <t>ANY</t>
-  </si>
-  <si>
     <t>{"split_faction": [X, X, X]}</t>
   </si>
   <si>
@@ -698,9 +692,6 @@
     <t>gray_and_black_tank</t>
   </si>
   <si>
-    <t>{"water_type": ["Seawater"]}</t>
-  </si>
-  <si>
     <t>agriculture,municipal_drinking</t>
   </si>
   <si>
@@ -710,20 +701,44 @@
     <t>Big_Spring_x</t>
   </si>
   <si>
-    <t>{"pass": "first" or "second", "feed_pressure": value}</t>
-  </si>
-  <si>
     <t>bar for pressure</t>
   </si>
   <si>
     <t>{"alum_dose" : 10, "polymer_dose": 0.1}</t>
+  </si>
+  <si>
+    <t>{"pass": "second", "membrane_area": 500000, "feed_pressure": 40, "type":"pass"}</t>
+  </si>
+  <si>
+    <t>ANY THAT HAS A SPLIT STREAM OUT - EXAMPLE IN PARAM DICT IS FOR 3 WAY SPLIT</t>
+  </si>
+  <si>
+    <t>cooling_tower</t>
+  </si>
+  <si>
+    <t>TO BE COMPLETED</t>
+  </si>
+  <si>
+    <t>{"pass": "first" or "second", "feed_pressure": value, "membrane_area": value}</t>
+  </si>
+  <si>
+    <t>membrane area only required for new RO method</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basic unit is a cost curve as a function of flow. </t>
+  </si>
+  <si>
+    <t>{"pass": "first", "membrane_area": 500000, "feed_pressure": 90, "type":"pass"}</t>
+  </si>
+  <si>
+    <t>{"water_type": ["seawater"]}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -761,12 +776,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
@@ -792,7 +801,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -803,7 +812,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1120,8 +1128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:N168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" topLeftCell="G21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1554,7 +1562,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>178</v>
       </c>
@@ -1580,10 +1588,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>178</v>
       </c>
@@ -1609,10 +1617,10 @@
         <v>163</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>178</v>
       </c>
@@ -1637,11 +1645,11 @@
       <c r="H19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="I19" s="8" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I19" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>178</v>
       </c>
@@ -1670,7 +1678,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>178</v>
       </c>
@@ -1699,7 +1707,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>178</v>
       </c>
@@ -1719,9 +1727,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>20</v>
@@ -1739,7 +1747,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1750,7 +1758,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>79</v>
       </c>
@@ -1779,7 +1787,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>79</v>
       </c>
@@ -1808,7 +1816,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -1837,7 +1845,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>79</v>
       </c>
@@ -1866,7 +1874,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>79</v>
       </c>
@@ -1886,7 +1894,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>79</v>
       </c>
@@ -1906,14 +1914,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="2" t="s">
@@ -1932,17 +1940,22 @@
         <v>0</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="2" t="s">
@@ -1961,17 +1974,22 @@
         <v>0</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+        <v>222</v>
+      </c>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D33" s="2" t="s">
@@ -1990,15 +2008,20 @@
         <v>35</v>
       </c>
       <c r="I33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D34" s="2" t="s">
@@ -2019,15 +2042,20 @@
       <c r="I34" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -2048,15 +2076,20 @@
       <c r="I35" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -2075,15 +2108,20 @@
         <v>0</v>
       </c>
       <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="2" t="s">
@@ -2102,17 +2140,22 @@
         <v>0</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+        <v>230</v>
+      </c>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="2" t="s">
@@ -2131,10 +2174,15 @@
         <v>0</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>21</v>
       </c>
@@ -2162,8 +2210,13 @@
       <c r="I39" s="2" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J39" s="2"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>21</v>
       </c>
@@ -2189,8 +2242,13 @@
         <v>0</v>
       </c>
       <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J40" s="2"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>21</v>
       </c>
@@ -2218,8 +2276,13 @@
       <c r="I41" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J41" s="2"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>21</v>
       </c>
@@ -2249,8 +2312,11 @@
       </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>21</v>
       </c>
@@ -2278,8 +2344,13 @@
       <c r="I43" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>21</v>
       </c>
@@ -2305,8 +2376,13 @@
         <v>35</v>
       </c>
       <c r="I44" s="2"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J44" s="2"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>21</v>
       </c>
@@ -2328,15 +2404,20 @@
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="C46" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D46" s="2" t="s">
@@ -2351,15 +2432,20 @@
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D47" s="2" t="s">
@@ -2374,8 +2460,13 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J47" s="2"/>
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="2"/>
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="D48" s="2"/>
@@ -4345,7 +4436,7 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>20</v>
@@ -4379,7 +4470,7 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>20</v>
@@ -4410,7 +4501,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>20</v>
@@ -4444,7 +4535,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B120" s="2" t="s">
         <v>20</v>
@@ -4476,7 +4567,7 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>20</v>
@@ -4510,7 +4601,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>20</v>
@@ -4544,7 +4635,7 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>20</v>
@@ -4567,7 +4658,7 @@
       <c r="H123" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I123" s="8" t="s">
+      <c r="I123" s="7" t="s">
         <v>207</v>
       </c>
       <c r="J123" s="2"/>
@@ -4578,7 +4669,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>20</v>
@@ -4612,7 +4703,7 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>20</v>
@@ -4646,7 +4737,7 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B126" s="2" t="s">
         <v>20</v>
@@ -4678,7 +4769,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B127" s="2" t="s">
         <v>20</v>
@@ -4712,7 +4803,7 @@
     </row>
     <row r="128" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A128" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B128" s="2" t="s">
         <v>20</v>
@@ -4746,7 +4837,7 @@
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A129" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B129" s="2" t="s">
         <v>20</v>
@@ -4778,7 +4869,7 @@
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A130" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B130" s="2" t="s">
         <v>20</v>
@@ -4834,7 +4925,7 @@
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>20</v>
@@ -4877,7 +4968,7 @@
         <v>25</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G134" s="3" t="s">
         <v>74</v>
@@ -4886,7 +4977,7 @@
         <v>0</v>
       </c>
       <c r="I134" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
@@ -4906,7 +4997,7 @@
         <v>25</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>65</v>
@@ -4915,7 +5006,7 @@
         <v>0</v>
       </c>
       <c r="I135" s="2" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J135" s="2"/>
       <c r="K135" s="2"/>
@@ -4943,7 +5034,7 @@
         <v>49</v>
       </c>
       <c r="G136" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H136" s="2" t="s">
         <v>163</v>
@@ -5862,10 +5953,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586A0CBC-F2B8-8D43-BF36-A9434BF68145}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection sqref="A1:D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5884,537 +5975,656 @@
       <c r="B1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>225</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>100</v>
+        <v>227</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>127</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>100</v>
+        <v>89</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>127</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>100</v>
+        <v>84</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>106</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>100</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>124</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>117</v>
-      </c>
+      <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>180</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>161</v>
-      </c>
+        <v>179</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>102</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C21" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>167</v>
-      </c>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>4</v>
+        <v>156</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>100</v>
+        <v>165</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="1"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>126</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C27" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D27" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="6"/>
-      <c r="B28" s="2" t="s">
-        <v>142</v>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="6"/>
       <c r="B29" s="2" t="s">
-        <v>195</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="2" t="s">
-        <v>96</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="2" t="s">
-        <v>134</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="B38" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
       <c r="B50" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="B52" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
       <c r="B53" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
       <c r="B54" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
       <c r="B55" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
       <c r="B56" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
       <c r="B57" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
       <c r="B58" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
       <c r="B59" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="6"/>
       <c r="B60" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
       <c r="B61" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="6"/>
       <c r="B62" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="6"/>
+      <c r="B63" s="2" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="2" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B64" s="2" t="s">
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B65" s="2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="2" t="s">
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B66" s="2" t="s">
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+    </row>
+    <row r="67" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B67" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D26">

</xml_diff>

<commit_message>
fixing ro methods to account for ERD and pump differences for stages/passes. added results saving and printing options.
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A59E41A7-3F4A-9C4B-A60E-F0BA7A317F49}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD1E264-1D87-0A41-BFE9-1187CDD71645}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13520" yWindow="1740" windowWidth="35640" windowHeight="23220" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="14940" yWindow="460" windowWidth="32200" windowHeight="20820" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1419" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1423" uniqueCount="234">
   <si>
     <t>outlet</t>
   </si>
@@ -707,31 +707,37 @@
     <t>{"alum_dose" : 10, "polymer_dose": 0.1}</t>
   </si>
   <si>
-    <t>{"pass": "second", "membrane_area": 500000, "feed_pressure": 40, "type":"pass"}</t>
-  </si>
-  <si>
     <t>ANY THAT HAS A SPLIT STREAM OUT - EXAMPLE IN PARAM DICT IS FOR 3 WAY SPLIT</t>
   </si>
   <si>
     <t>cooling_tower</t>
   </si>
   <si>
-    <t>TO BE COMPLETED</t>
-  </si>
-  <si>
-    <t>{"pass": "first" or "second", "feed_pressure": value, "membrane_area": value}</t>
-  </si>
-  <si>
-    <t>membrane area only required for new RO method</t>
-  </si>
-  <si>
     <t xml:space="preserve">Basic unit is a cost curve as a function of flow. </t>
   </si>
   <si>
-    <t>{"pass": "first", "membrane_area": 500000, "feed_pressure": 90, "type":"pass"}</t>
-  </si>
-  <si>
     <t>{"water_type": ["seawater"]}</t>
+  </si>
+  <si>
+    <t>{"cost_type": "first" or "second", "feed_pressure": value, "type": "pass" or "stage", "erd": "yes" or "no"}</t>
+  </si>
+  <si>
+    <t>{"feed_pressure": value, "membrane_area": value, "type": "pass" or "stage", "erd": "yes" or "no"}</t>
+  </si>
+  <si>
+    <t>bar for pressure, m2 for area</t>
+  </si>
+  <si>
+    <t>See Word Document for cooling tower</t>
+  </si>
+  <si>
+    <t>ERD Setting is important and user can input wrong value if not careful</t>
+  </si>
+  <si>
+    <t>{"pass": "first", "membrane_area": 500000, "feed_pressure": 85, "type":"pass", "erd": "yes"}</t>
+  </si>
+  <si>
+    <t>{"pass": "second", "membrane_area": 500000, "feed_pressure": 35, "type":"pass", "erd": "yes"}</t>
   </si>
 </sst>
 </file>
@@ -1128,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:N168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1940,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
@@ -2140,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="I37" s="7" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
@@ -2174,7 +2180,7 @@
         <v>0</v>
       </c>
       <c r="I38" s="7" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
@@ -5953,10 +5959,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586A0CBC-F2B8-8D43-BF36-A9434BF68145}">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D67"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5984,7 +5990,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>210</v>
@@ -5998,16 +6004,16 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -6021,148 +6027,150 @@
         <v>221</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>203</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>228</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="1"/>
+        <v>229</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>127</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>104</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>80</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>127</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>80</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>158</v>
+        <v>84</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" s="1"/>
+        <v>116</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>50</v>
+        <v>158</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>124</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>107</v>
+        <v>157</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>119</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>86</v>
+        <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>85</v>
@@ -6174,94 +6182,94 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>179</v>
+        <v>85</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>180</v>
+        <v>117</v>
       </c>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>39</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="C18" s="1"/>
+        <v>179</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>180</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>102</v>
-      </c>
+        <v>161</v>
+      </c>
+      <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>168</v>
+        <v>108</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>88</v>
+        <v>168</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>156</v>
+        <v>87</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>165</v>
+        <v>88</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>167</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>4</v>
+        <v>156</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>101</v>
+        <v>165</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="D23" s="1"/>
+        <v>166</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>100</v>
@@ -6270,66 +6278,70 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="D25" s="1"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>126</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C28" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="6"/>
-      <c r="B29" s="2" t="s">
-        <v>142</v>
-      </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
+      <c r="D29" s="1" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="6"/>
       <c r="B30" s="2" t="s">
-        <v>195</v>
+        <v>142</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -6337,7 +6349,7 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="6"/>
       <c r="B31" s="2" t="s">
-        <v>96</v>
+        <v>195</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
@@ -6345,7 +6357,7 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="6"/>
       <c r="B32" s="2" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -6353,7 +6365,7 @@
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="6"/>
       <c r="B33" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -6361,7 +6373,7 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="6"/>
       <c r="B34" s="2" t="s">
-        <v>186</v>
+        <v>139</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -6369,7 +6381,7 @@
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="6"/>
       <c r="B35" s="2" t="s">
-        <v>98</v>
+        <v>186</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
@@ -6377,7 +6389,7 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="6"/>
       <c r="B36" s="2" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
@@ -6385,7 +6397,7 @@
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="6"/>
       <c r="B37" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
@@ -6393,7 +6405,7 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="6"/>
       <c r="B38" s="2" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
@@ -6401,7 +6413,7 @@
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="6"/>
       <c r="B39" s="2" t="s">
-        <v>144</v>
+        <v>154</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
@@ -6409,7 +6421,7 @@
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="6"/>
       <c r="B40" s="2" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -6417,7 +6429,7 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
       <c r="B41" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -6425,7 +6437,7 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
       <c r="B42" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
@@ -6433,7 +6445,7 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="6"/>
       <c r="B43" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
@@ -6441,7 +6453,7 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="6"/>
       <c r="B44" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
@@ -6449,7 +6461,7 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="6"/>
       <c r="B45" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -6457,7 +6469,7 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="6"/>
       <c r="B46" s="2" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
@@ -6465,7 +6477,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="6"/>
       <c r="B47" s="2" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
@@ -6473,7 +6485,7 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="6"/>
       <c r="B48" s="2" t="s">
-        <v>152</v>
+        <v>39</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -6481,7 +6493,7 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="6"/>
       <c r="B49" s="2" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
@@ -6489,7 +6501,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="6"/>
       <c r="B50" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -6497,7 +6509,7 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="6"/>
       <c r="B51" s="2" t="s">
-        <v>65</v>
+        <v>132</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -6505,7 +6517,7 @@
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="6"/>
       <c r="B52" s="2" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
@@ -6513,7 +6525,7 @@
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="6"/>
       <c r="B53" s="2" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -6521,7 +6533,7 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="6"/>
       <c r="B54" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
@@ -6529,7 +6541,7 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="6"/>
       <c r="B55" s="2" t="s">
-        <v>90</v>
+        <v>137</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
@@ -6537,7 +6549,7 @@
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="6"/>
       <c r="B56" s="2" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
@@ -6545,7 +6557,7 @@
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="6"/>
       <c r="B57" s="2" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -6553,7 +6565,7 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="6"/>
       <c r="B58" s="2" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
@@ -6561,7 +6573,7 @@
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="6"/>
       <c r="B59" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -6569,7 +6581,7 @@
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="6"/>
       <c r="B60" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -6577,7 +6589,7 @@
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="6"/>
       <c r="B61" s="2" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -6585,7 +6597,7 @@
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="6"/>
       <c r="B62" s="2" t="s">
-        <v>147</v>
+        <v>171</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -6593,42 +6605,50 @@
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="6"/>
       <c r="B63" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="6"/>
       <c r="B64" s="2" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="2" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="2" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
     </row>
+    <row r="68" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B68" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D26">
-    <sortCondition ref="A1:A26"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:D27">
+    <sortCondition ref="A1:A27"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixing RO and running SB + TB
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E694A2E-4DD2-0C49-8B04-C86B0536AA92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97EE41B-B32C-A44F-9E6F-072101761331}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18040" yWindow="1660" windowWidth="32200" windowHeight="20820" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="13400" yWindow="3660" windowWidth="32200" windowHeight="20820" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="185">
   <si>
     <t>outlet</t>
   </si>
@@ -584,10 +584,13 @@
     <t>lime_softening,ro_first_pass</t>
   </si>
   <si>
-    <t>{'type': 'pass', "pass": "first", "membrane_area": 500000, "feed_pressure": 85, 'erd': 'yes',  'split_fraction': [0.67, 0.33]}</t>
-  </si>
-  <si>
-    <t>{'type': 'pass', "pass": "second", "membrane_area": 500000, "feed_pressure": 35, 'erd': 'yes'}</t>
+    <t>{'pump': 'yes', 'type': 'pass', "pass": "second", "membrane_area": 500000, "feed_pressure": 35, 'erd': 'yes'}</t>
+  </si>
+  <si>
+    <t>{'pump': 'yes', 'type': 'pass', "pass": "first", "membrane_area": 500000, "feed_pressure": 85, 'erd': 'yes',  'split_fraction': [0.67, 0.33]}</t>
+  </si>
+  <si>
+    <t>{"pass": "first", "membrane_area": 500000, "feed_pressure": 85, "type":"pass", "erd": "yes", "pump":"yes"}</t>
   </si>
 </sst>
 </file>
@@ -991,8 +994,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G27" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1292,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="I10" s="7" t="s">
-        <v>160</v>
+        <v>184</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -2328,7 +2331,7 @@
         <v>131</v>
       </c>
       <c r="I46" s="8" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -2357,7 +2360,7 @@
         <v>32</v>
       </c>
       <c r="I47" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
trying to fix master2
</commit_message>
<xml_diff>
--- a/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
+++ b/IDAES-WaterTAP3_v2/data/case_study_train_input_test.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amiara/NAWI/WaterTap/NAWI-WaterTAP3/IDAES-WaterTAP3_v2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E97EE41B-B32C-A44F-9E6F-072101761331}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC15269D-8112-9E44-B622-E8EBA8CD6151}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="3660" windowWidth="32200" windowHeight="20820" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
+    <workbookView xWindow="5320" yWindow="1360" windowWidth="35660" windowHeight="18960" xr2:uid="{5688C9C7-4B8A-264D-AE07-643E0DA37154}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="2" r:id="rId1"/>
     <sheet name="parameters" sheetId="3" r:id="rId2"/>
     <sheet name="general notes" sheetId="4" r:id="rId3"/>
+    <sheet name="To Do" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="235">
   <si>
     <t>outlet</t>
   </si>
@@ -591,13 +592,163 @@
   </si>
   <si>
     <t>{"pass": "first", "membrane_area": 500000, "feed_pressure": 85, "type":"pass", "erd": "yes", "pump":"yes"}</t>
+  </si>
+  <si>
+    <t>heap_leaching</t>
+  </si>
+  <si>
+    <t>agglom_stacking</t>
+  </si>
+  <si>
+    <t>{"water_type": ["ore_heap_make_up", "well_field"]}</t>
+  </si>
+  <si>
+    <t>solution_distribution_and_recovery_plant</t>
+  </si>
+  <si>
+    <t>industrial</t>
+  </si>
+  <si>
+    <t>{"unit_process_name":"industrial"}</t>
+  </si>
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
+    <t>Where does heap leaching waste go?</t>
+  </si>
+  <si>
+    <t>Resolved</t>
+  </si>
+  <si>
+    <t>Case study</t>
+  </si>
+  <si>
+    <t>heap leaching</t>
+  </si>
+  <si>
+    <t>big_spring</t>
+  </si>
+  <si>
+    <t>onsite_storage</t>
+  </si>
+  <si>
+    <t>{"water_type": ["big_spring_feed"], 'unit_process_name': 'onsite_storage'}</t>
+  </si>
+  <si>
+    <t>reverse_osmosis,uv_aop</t>
+  </si>
+  <si>
+    <t>{"unit_process_name": 'microfiltration', 'split_fraction': [0.75, 0.25]}</t>
+  </si>
+  <si>
+    <t>{"pass": "first", "membrane_area": 500000, "feed_pressure": 85, 'type': 'pass', 'erd': 'yes', 'pump': 'yes'}</t>
+  </si>
+  <si>
+    <t>{"chemical_name": ["Hydrogen_Peroxide"], 'dose': 5, "uv_dose": 100, 'aop': True, 'uvt_in': 0.95}</t>
+  </si>
+  <si>
+    <t>{'hours': 6}</t>
+  </si>
+  <si>
+    <t>emwd</t>
+  </si>
+  <si>
+    <t>well_field</t>
+  </si>
+  <si>
+    <t>iron_and_manganese_removal</t>
+  </si>
+  <si>
+    <t>{"water_type": ["emwd_ca_brackish"]}</t>
+  </si>
+  <si>
+    <t>outlet,outlet,outlet</t>
+  </si>
+  <si>
+    <t>{'split_fraction': [0.333, 0.333, 0.334]}</t>
+  </si>
+  <si>
+    <t>cartridge_filtration_a</t>
+  </si>
+  <si>
+    <t>ro_1</t>
+  </si>
+  <si>
+    <t>ro_brine_1</t>
+  </si>
+  <si>
+    <t>cartridge_filtration_b</t>
+  </si>
+  <si>
+    <t>ro_2</t>
+  </si>
+  <si>
+    <t>chlorination,ro_brine_2</t>
+  </si>
+  <si>
+    <t>ro_brine_2</t>
+  </si>
+  <si>
+    <t>{"hours": 3}</t>
+  </si>
+  <si>
+    <t>{'pump': 'yes', 'type': 'pass', "pass": "first", "membrane_area": 500000, "feed_pressure": 85, 'erd': 'yes'}</t>
+  </si>
+  <si>
+    <t>{'pump': 'yes', 'type': 'pass', "pass": "second", "membrane_area": 500000, "feed_pressure": 85, 'erd': 'yes'}</t>
+  </si>
+  <si>
+    <t>emwd_x</t>
+  </si>
+  <si>
+    <t>{'pump': 'yes', 'type': 'stage', "pass": "second", "membrane_area": 500000, "feed_pressure": 85, 'erd': 'yes'}</t>
+  </si>
+  <si>
+    <t>{'pump': 'yes', 'type': 'pass', "pass": "first", "membrane_area": 500000, "feed_pressure": 85, 'erd': 'no'}</t>
+  </si>
+  <si>
+    <t>hrsd</t>
+  </si>
+  <si>
+    <t>{"water_type": ["hrsd_municipal"], "pump_type": "raw", 'tdh': 125}</t>
+  </si>
+  <si>
+    <t>{"chemical_name": ["Iron_FeCl3"], "dose": 30}</t>
+  </si>
+  <si>
+    <t>fixed_bed_gravity_basin</t>
+  </si>
+  <si>
+    <t>uv_aop,sludge_tank</t>
+  </si>
+  <si>
+    <t>{'ebct': 30}</t>
+  </si>
+  <si>
+    <t>{"chemical_name": ["Hydrogen_Peroxide"], 'dose': 5, "uv_dose": 80, 'aop': False, 'uvt_in': 0.8}</t>
+  </si>
+  <si>
+    <t>{"hours": 6}</t>
+  </si>
+  <si>
+    <t>{"unit_process_name": 'recharge_pump_well'}</t>
+  </si>
+  <si>
+    <t>{"unit_process_name": 'sludge_tank'}</t>
+  </si>
+  <si>
+    <t>hrsd_x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -645,6 +796,18 @@
       <name val="Consolas"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -666,7 +829,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -678,6 +841,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -992,10 +1157,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A817730-1204-A546-BE57-7C8F485A64DC}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:Z95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D84" sqref="D84:F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2392,7 +2557,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>175</v>
       </c>
@@ -2421,7 +2586,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>175</v>
       </c>
@@ -2450,7 +2615,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>175</v>
       </c>
@@ -2479,7 +2644,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>175</v>
       </c>
@@ -2508,7 +2673,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>175</v>
       </c>
@@ -2537,7 +2702,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>175</v>
       </c>
@@ -2560,7 +2725,7 @@
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>175</v>
       </c>
@@ -2582,6 +2747,1550 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A57" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F57" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="J57" s="2"/>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I58" s="2"/>
+      <c r="J58" s="2"/>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A59" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+      <c r="M59" s="2"/>
+      <c r="N59" s="2"/>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A60" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="J60" s="2"/>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+    </row>
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A61" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A63" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="G63" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H63" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I63" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="J63"/>
+      <c r="K63"/>
+      <c r="L63"/>
+      <c r="M63"/>
+      <c r="N63"/>
+      <c r="O63"/>
+      <c r="P63"/>
+      <c r="Q63"/>
+      <c r="R63"/>
+      <c r="S63"/>
+      <c r="T63"/>
+      <c r="U63"/>
+      <c r="V63"/>
+      <c r="W63"/>
+      <c r="X63"/>
+      <c r="Y63"/>
+      <c r="Z63"/>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A64" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C64" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D64" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="H64" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+      <c r="N64"/>
+      <c r="O64"/>
+      <c r="P64"/>
+      <c r="Q64"/>
+      <c r="R64"/>
+      <c r="S64"/>
+      <c r="T64"/>
+      <c r="U64"/>
+      <c r="V64"/>
+      <c r="W64"/>
+      <c r="X64"/>
+      <c r="Y64"/>
+      <c r="Z64"/>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A65" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C65" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D65" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="G65" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I65" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="J65"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="O65"/>
+      <c r="P65"/>
+      <c r="Q65"/>
+      <c r="R65"/>
+      <c r="S65"/>
+      <c r="T65"/>
+      <c r="U65"/>
+      <c r="V65"/>
+      <c r="W65"/>
+      <c r="X65"/>
+      <c r="Y65"/>
+      <c r="Z65"/>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A66" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H66" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I66" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66"/>
+      <c r="P66"/>
+      <c r="Q66"/>
+      <c r="R66"/>
+      <c r="S66"/>
+      <c r="T66"/>
+      <c r="U66"/>
+      <c r="V66"/>
+      <c r="W66"/>
+      <c r="X66"/>
+      <c r="Y66"/>
+      <c r="Z66"/>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A67" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C67" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G67" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I67" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="J67"/>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67"/>
+      <c r="P67"/>
+      <c r="Q67"/>
+      <c r="R67"/>
+      <c r="S67"/>
+      <c r="T67"/>
+      <c r="U67"/>
+      <c r="V67"/>
+      <c r="W67"/>
+      <c r="X67"/>
+      <c r="Y67"/>
+      <c r="Z67"/>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A68" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68"/>
+      <c r="H68"/>
+      <c r="I68"/>
+      <c r="J68"/>
+      <c r="K68"/>
+      <c r="L68"/>
+      <c r="M68"/>
+      <c r="N68"/>
+      <c r="O68"/>
+      <c r="P68"/>
+      <c r="Q68"/>
+      <c r="R68"/>
+      <c r="S68"/>
+      <c r="T68"/>
+      <c r="U68"/>
+      <c r="V68"/>
+      <c r="W68"/>
+      <c r="X68"/>
+      <c r="Y68"/>
+      <c r="Z68"/>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A69" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C69" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G69"/>
+      <c r="H69"/>
+      <c r="I69"/>
+      <c r="J69"/>
+      <c r="K69"/>
+      <c r="L69"/>
+      <c r="M69"/>
+      <c r="N69"/>
+      <c r="O69"/>
+      <c r="P69"/>
+      <c r="Q69"/>
+      <c r="R69"/>
+      <c r="S69"/>
+      <c r="T69"/>
+      <c r="U69"/>
+      <c r="V69"/>
+      <c r="W69"/>
+      <c r="X69"/>
+      <c r="Y69"/>
+      <c r="Z69"/>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A71" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D71" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="E71" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="H71" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I71" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="J71"/>
+      <c r="K71"/>
+      <c r="L71"/>
+      <c r="M71"/>
+      <c r="N71"/>
+      <c r="O71"/>
+      <c r="P71"/>
+      <c r="Q71"/>
+      <c r="R71"/>
+      <c r="S71"/>
+      <c r="T71"/>
+      <c r="U71"/>
+      <c r="V71"/>
+      <c r="W71"/>
+      <c r="X71"/>
+      <c r="Y71"/>
+      <c r="Z71"/>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A72" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B72" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C72" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D72" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="E72" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="G72" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="H72" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="I72" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="J72"/>
+      <c r="K72"/>
+      <c r="L72"/>
+      <c r="M72"/>
+      <c r="N72"/>
+      <c r="O72"/>
+      <c r="P72"/>
+      <c r="Q72"/>
+      <c r="R72"/>
+      <c r="S72"/>
+      <c r="T72"/>
+      <c r="U72"/>
+      <c r="V72"/>
+      <c r="W72"/>
+      <c r="X72"/>
+      <c r="Y72"/>
+      <c r="Z72"/>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A73" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F73" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="H73" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I73"/>
+      <c r="J73"/>
+      <c r="K73"/>
+      <c r="L73"/>
+      <c r="M73"/>
+      <c r="N73"/>
+      <c r="O73"/>
+      <c r="P73"/>
+      <c r="Q73"/>
+      <c r="R73"/>
+      <c r="S73"/>
+      <c r="T73"/>
+      <c r="U73"/>
+      <c r="V73"/>
+      <c r="W73"/>
+      <c r="X73"/>
+      <c r="Y73"/>
+      <c r="Z73"/>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A74" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D74" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F74" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="G74" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I74" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="J74"/>
+      <c r="K74"/>
+      <c r="L74"/>
+      <c r="M74"/>
+      <c r="N74"/>
+      <c r="O74"/>
+      <c r="P74"/>
+      <c r="Q74"/>
+      <c r="R74"/>
+      <c r="S74"/>
+      <c r="T74"/>
+      <c r="U74"/>
+      <c r="V74"/>
+      <c r="W74"/>
+      <c r="X74"/>
+      <c r="Y74"/>
+      <c r="Z74"/>
+    </row>
+    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A75" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F75" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="G75" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H75" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I75" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="J75"/>
+      <c r="K75"/>
+      <c r="L75"/>
+      <c r="M75"/>
+      <c r="N75"/>
+      <c r="O75"/>
+      <c r="P75"/>
+      <c r="Q75"/>
+      <c r="R75"/>
+      <c r="S75"/>
+      <c r="T75"/>
+      <c r="U75"/>
+      <c r="V75"/>
+      <c r="W75"/>
+      <c r="X75"/>
+      <c r="Y75"/>
+      <c r="Z75"/>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A76" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="G76" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I76"/>
+      <c r="J76"/>
+      <c r="K76"/>
+      <c r="L76"/>
+      <c r="M76"/>
+      <c r="N76"/>
+      <c r="O76"/>
+      <c r="P76"/>
+      <c r="Q76"/>
+      <c r="R76"/>
+      <c r="S76"/>
+      <c r="T76"/>
+      <c r="U76"/>
+      <c r="V76"/>
+      <c r="W76"/>
+      <c r="X76"/>
+      <c r="Y76"/>
+      <c r="Z76"/>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A77" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D77" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F77" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="G77" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="H77" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I77" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="J77"/>
+      <c r="K77"/>
+      <c r="L77"/>
+      <c r="M77"/>
+      <c r="N77"/>
+      <c r="O77"/>
+      <c r="P77"/>
+      <c r="Q77"/>
+      <c r="R77"/>
+      <c r="S77"/>
+      <c r="T77"/>
+      <c r="U77"/>
+      <c r="V77"/>
+      <c r="W77"/>
+      <c r="X77"/>
+      <c r="Y77"/>
+      <c r="Z77"/>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A78" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D78" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F78" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="G78" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I78" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="J78"/>
+      <c r="K78"/>
+      <c r="L78"/>
+      <c r="M78"/>
+      <c r="N78"/>
+      <c r="O78"/>
+      <c r="P78"/>
+      <c r="Q78"/>
+      <c r="R78"/>
+      <c r="S78"/>
+      <c r="T78"/>
+      <c r="U78"/>
+      <c r="V78"/>
+      <c r="W78"/>
+      <c r="X78"/>
+      <c r="Y78"/>
+      <c r="Z78"/>
+    </row>
+    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A79" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B79" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C79" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D79" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E79" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F79" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H79" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I79" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J79"/>
+      <c r="K79"/>
+      <c r="L79"/>
+      <c r="M79"/>
+      <c r="N79"/>
+      <c r="O79"/>
+      <c r="P79"/>
+      <c r="Q79"/>
+      <c r="R79"/>
+      <c r="S79"/>
+      <c r="T79"/>
+      <c r="U79"/>
+      <c r="V79"/>
+      <c r="W79"/>
+      <c r="X79"/>
+      <c r="Y79"/>
+      <c r="Z79"/>
+    </row>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A80" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B80" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C80" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D80" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E80" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F80" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G80" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H80" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I80" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="J80"/>
+      <c r="K80"/>
+      <c r="L80"/>
+      <c r="M80"/>
+      <c r="N80"/>
+      <c r="O80"/>
+      <c r="P80"/>
+      <c r="Q80"/>
+      <c r="R80"/>
+      <c r="S80"/>
+      <c r="T80"/>
+      <c r="U80"/>
+      <c r="V80"/>
+      <c r="W80"/>
+      <c r="X80"/>
+      <c r="Y80"/>
+      <c r="Z80"/>
+    </row>
+    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A81" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B81" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C81" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D81" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F81" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G81"/>
+      <c r="H81"/>
+      <c r="I81"/>
+      <c r="J81"/>
+      <c r="K81"/>
+      <c r="L81"/>
+      <c r="M81"/>
+      <c r="N81"/>
+      <c r="O81"/>
+      <c r="P81"/>
+      <c r="Q81"/>
+      <c r="R81"/>
+      <c r="S81"/>
+      <c r="T81"/>
+      <c r="U81"/>
+      <c r="V81"/>
+      <c r="W81"/>
+      <c r="X81"/>
+      <c r="Y81"/>
+      <c r="Z81"/>
+    </row>
+    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A82" s="8" t="s">
+        <v>221</v>
+      </c>
+      <c r="B82" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D82" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E82" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F82" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G82"/>
+      <c r="H82"/>
+      <c r="I82"/>
+      <c r="J82"/>
+      <c r="K82"/>
+      <c r="L82"/>
+      <c r="M82"/>
+      <c r="N82"/>
+      <c r="O82"/>
+      <c r="P82"/>
+      <c r="Q82"/>
+      <c r="R82"/>
+      <c r="S82"/>
+      <c r="T82"/>
+      <c r="U82"/>
+      <c r="V82"/>
+      <c r="W82"/>
+      <c r="X82"/>
+      <c r="Y82"/>
+      <c r="Z82"/>
+    </row>
+    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A84" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C84" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G84" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H84" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I84" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="J84"/>
+      <c r="K84"/>
+      <c r="L84"/>
+      <c r="M84"/>
+      <c r="N84"/>
+      <c r="O84"/>
+      <c r="P84"/>
+      <c r="Q84"/>
+      <c r="R84"/>
+      <c r="S84"/>
+      <c r="T84"/>
+      <c r="U84"/>
+      <c r="V84"/>
+      <c r="W84"/>
+      <c r="X84"/>
+      <c r="Y84"/>
+      <c r="Z84"/>
+    </row>
+    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A85" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B85" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D85" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E85" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I85" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="J85"/>
+      <c r="K85"/>
+      <c r="L85"/>
+      <c r="M85"/>
+      <c r="N85"/>
+      <c r="O85"/>
+      <c r="P85"/>
+      <c r="Q85"/>
+      <c r="R85"/>
+      <c r="S85"/>
+      <c r="T85"/>
+      <c r="U85"/>
+      <c r="V85"/>
+      <c r="W85"/>
+      <c r="X85"/>
+      <c r="Y85"/>
+      <c r="Z85"/>
+    </row>
+    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A86" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B86" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C86" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D86" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E86" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F86" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G86" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="H86" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I86" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="J86"/>
+      <c r="K86"/>
+      <c r="L86"/>
+      <c r="M86"/>
+      <c r="N86"/>
+      <c r="O86"/>
+      <c r="P86"/>
+      <c r="Q86"/>
+      <c r="R86"/>
+      <c r="S86"/>
+      <c r="T86"/>
+      <c r="U86"/>
+      <c r="V86"/>
+      <c r="W86"/>
+      <c r="X86"/>
+      <c r="Y86"/>
+      <c r="Z86"/>
+    </row>
+    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A87" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B87" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E87" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F87" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="G87" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H87" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I87" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="J87"/>
+      <c r="K87"/>
+      <c r="L87"/>
+      <c r="M87"/>
+      <c r="N87"/>
+      <c r="O87"/>
+      <c r="P87"/>
+      <c r="Q87"/>
+      <c r="R87"/>
+      <c r="S87"/>
+      <c r="T87"/>
+      <c r="U87"/>
+      <c r="V87"/>
+      <c r="W87"/>
+      <c r="X87"/>
+      <c r="Y87"/>
+      <c r="Z87"/>
+    </row>
+    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A88" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B88" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C88" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D88" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E88" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F88" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G88" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="H88" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I88" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="J88"/>
+      <c r="K88"/>
+      <c r="L88"/>
+      <c r="M88"/>
+      <c r="N88"/>
+      <c r="O88"/>
+      <c r="P88"/>
+      <c r="Q88"/>
+      <c r="R88"/>
+      <c r="S88"/>
+      <c r="T88"/>
+      <c r="U88"/>
+      <c r="V88"/>
+      <c r="W88"/>
+      <c r="X88"/>
+      <c r="Y88"/>
+      <c r="Z88"/>
+    </row>
+    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A89" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B89" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F89" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="G89" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H89" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I89"/>
+      <c r="J89"/>
+      <c r="K89"/>
+      <c r="L89"/>
+      <c r="M89"/>
+      <c r="N89"/>
+      <c r="O89"/>
+      <c r="P89"/>
+      <c r="Q89"/>
+      <c r="R89"/>
+      <c r="S89"/>
+      <c r="T89"/>
+      <c r="U89"/>
+      <c r="V89"/>
+      <c r="W89"/>
+      <c r="X89"/>
+      <c r="Y89"/>
+      <c r="Z89"/>
+    </row>
+    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A90" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B90" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C90" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D90" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E90" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F90" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I90" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="J90"/>
+      <c r="K90"/>
+      <c r="L90"/>
+      <c r="M90"/>
+      <c r="N90"/>
+      <c r="O90"/>
+      <c r="P90"/>
+      <c r="Q90"/>
+      <c r="R90"/>
+      <c r="S90"/>
+      <c r="T90"/>
+      <c r="U90"/>
+      <c r="V90"/>
+      <c r="W90"/>
+      <c r="X90"/>
+      <c r="Y90"/>
+      <c r="Z90"/>
+    </row>
+    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A91" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B91" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C91" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D91" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E91" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F91" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G91" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H91" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I91" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="J91"/>
+      <c r="K91"/>
+      <c r="L91"/>
+      <c r="M91"/>
+      <c r="N91"/>
+      <c r="O91"/>
+      <c r="P91"/>
+      <c r="Q91"/>
+      <c r="R91"/>
+      <c r="S91"/>
+      <c r="T91"/>
+      <c r="U91"/>
+      <c r="V91"/>
+      <c r="W91"/>
+      <c r="X91"/>
+      <c r="Y91"/>
+      <c r="Z91"/>
+    </row>
+    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A92" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B92" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C92" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D92" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="E92" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F92" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="G92" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H92" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I92" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="J92"/>
+      <c r="K92"/>
+      <c r="L92"/>
+      <c r="M92"/>
+      <c r="N92"/>
+      <c r="O92"/>
+      <c r="P92"/>
+      <c r="Q92"/>
+      <c r="R92"/>
+      <c r="S92"/>
+      <c r="T92"/>
+      <c r="U92"/>
+      <c r="V92"/>
+      <c r="W92"/>
+      <c r="X92"/>
+      <c r="Y92"/>
+      <c r="Z92"/>
+    </row>
+    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A93" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D93" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E93" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F93" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G93" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="H93" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I93" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="J93"/>
+      <c r="K93"/>
+      <c r="L93"/>
+      <c r="M93"/>
+      <c r="N93"/>
+      <c r="O93"/>
+      <c r="P93"/>
+      <c r="Q93"/>
+      <c r="R93"/>
+      <c r="S93"/>
+      <c r="T93"/>
+      <c r="U93"/>
+      <c r="V93"/>
+      <c r="W93"/>
+      <c r="X93"/>
+      <c r="Y93"/>
+      <c r="Z93"/>
+    </row>
+    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A94" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B94" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C94" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D94" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E94" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F94" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G94"/>
+      <c r="H94"/>
+      <c r="I94" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="J94"/>
+      <c r="K94"/>
+      <c r="L94"/>
+      <c r="M94"/>
+      <c r="N94"/>
+      <c r="O94"/>
+      <c r="P94"/>
+      <c r="Q94"/>
+      <c r="R94"/>
+      <c r="S94"/>
+      <c r="T94"/>
+      <c r="U94"/>
+      <c r="V94"/>
+      <c r="W94"/>
+      <c r="X94"/>
+      <c r="Y94"/>
+      <c r="Z94"/>
+    </row>
+    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A95" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B95" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E95" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F95" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G95"/>
+      <c r="H95"/>
+      <c r="I95" s="10" t="s">
+        <v>233</v>
+      </c>
+      <c r="J95"/>
+      <c r="K95"/>
+      <c r="L95"/>
+      <c r="M95"/>
+      <c r="N95"/>
+      <c r="O95"/>
+      <c r="P95"/>
+      <c r="Q95"/>
+      <c r="R95"/>
+      <c r="S95"/>
+      <c r="T95"/>
+      <c r="U95"/>
+      <c r="V95"/>
+      <c r="W95"/>
+      <c r="X95"/>
+      <c r="Y95"/>
+      <c r="Z95"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I39">
@@ -3324,4 +5033,46 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85BB9832-4A71-B84F-BEAB-4595D9EE31AA}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>